<commit_message>
Finished pulling code snippets from Lynis
</commit_message>
<xml_diff>
--- a/Priv Esc Checks/LynisModules.xlsx
+++ b/Priv Esc Checks/LynisModules.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="710" firstSheet="22" activeTab="27"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="710" firstSheet="36" activeTab="42"/>
   </bookViews>
   <sheets>
     <sheet name="binaries" sheetId="1" r:id="rId1"/>
@@ -40,6 +40,21 @@
     <sheet name="networking" sheetId="26" r:id="rId26"/>
     <sheet name="php" sheetId="27" r:id="rId27"/>
     <sheet name="ports_packages" sheetId="28" r:id="rId28"/>
+    <sheet name="printers_spools" sheetId="29" r:id="rId29"/>
+    <sheet name="scheduling" sheetId="30" r:id="rId30"/>
+    <sheet name="shells" sheetId="31" r:id="rId31"/>
+    <sheet name="snmp" sheetId="32" r:id="rId32"/>
+    <sheet name="squid" sheetId="33" r:id="rId33"/>
+    <sheet name="ssh" sheetId="34" r:id="rId34"/>
+    <sheet name="storage" sheetId="35" r:id="rId35"/>
+    <sheet name="storage_nfs" sheetId="36" r:id="rId36"/>
+    <sheet name="system_integrity" sheetId="37" r:id="rId37"/>
+    <sheet name="time" sheetId="38" r:id="rId38"/>
+    <sheet name="tooling" sheetId="39" r:id="rId39"/>
+    <sheet name="USB" sheetId="40" r:id="rId40"/>
+    <sheet name="virtualization" sheetId="41" r:id="rId41"/>
+    <sheet name="webservers" sheetId="42" r:id="rId42"/>
+    <sheet name="tips" sheetId="43" r:id="rId43"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -51,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1189" uniqueCount="1149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="1324">
   <si>
     <t xml:space="preserve"> aa-status (apparmor component) - ${BINARY}" ;;</t>
   </si>
@@ -12461,6 +12476,3381 @@
                 LogText "Result: found ${KERNELS} on the system, which is fine"
                 AddHP 1 1
             fi
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>printcap file consistency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : PRNT-2302
+    # Description : Check printcap file consistency
+    Register --test-no PRNT-2302 --os FreeBSD --weight L --network NO --category security --description "Check for printcap consistency"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Searching /usr/sbin/chkprintcap"
+        if [ ! -f ${ROOTDIR}usr/sbin/chkprintcap ]; then
+            Display --indent 2 --text "- Checking chkprintcap" --result "${STATUS_NOT_FOUND}" --color WHITE
+            LogText "Result: ${ROOTDIR}usr/sbin/chkprintcap NOT found, test skipped"
+        else
+            LogText "Result: ${ROOTDIR}usr/sbin/chkprintcap found"
+            FIND=$(${ROOTDIR}usr/sbin/chkprintcap &gt; /dev/null ; echo $?)
+            # Only an exit code of zero should come back. Use string instead of integer, due unexpected trash
+            if [ "${FIND}" = "0" ]; then
+                Display --indent 2 --text "- Integrity check of printcap file" --result "${STATUS_OK}" --color GREEN
+                LogText "Result: chkprintcap did NOT gave any warnings"
+            else
+                Display --indent 2 --text "- Integrity check of printcap file" --result "${STATUS_WARNING}" --color RED
+                ReportSuggestion ${TEST_NO} "Run chkprintcap manually to test printcap file"
+                LogText "Output from chkprintcap: ${FIND}"
+                LogText "Run chkprintcap and check the ${ROOTDIR}etc/printcap file"
+            fi
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>cupsd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : PRNT-2304
+    # Description : Check cupsd status
+    Register --test-no PRNT-2304 --weight L --network NO --category security --description "Check cupsd status"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking cupsd status"
+        IsRunning cupsd
+        if [ ${RUNNING} -eq 1 ]; then
+            Display --indent 2 --text "- Checking cups daemon" --result "${STATUS_RUNNING}" --color GREEN
+            LogText "Result: cups daemon running"
+            CUPSD_RUNNING=1; PRINTING_DAEMON="cups"
+        else
+            Display --indent 2 --text "- Checking cups daemon" --result "${STATUS_NOT_FOUND}" --color WHITE
+            LogText "Result: cups daemon not running, cups daemon tests skipped"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : PRNT-2306
+    # Description : Check CUPSd configuration file
+    if [ ${CUPSD_RUNNING} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no PRNT-2306 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check CUPSd configuration file"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Searching cupsd configuration file"
+        for DIR in ${CUPSD_CONFIG_LOCS}; do
+            if [ -f ${DIR}/cupsd.conf ]; then
+                if FileIsReadable ${DIR}/cupsd.conf; then
+                    CUPSD_CONFIG_FILE="${DIR}/cupsd.conf"
+                    LogText "Result: found ${CUPSD_CONFIG_FILE}"
+                fi
+            fi
+        done
+        if HasData "${CUPSD_CONFIG_FILE}"; then
+            Display --indent 2 --text "- Checking CUPS configuration file" --result "${STATUS_OK}" --color GREEN
+            LogText "Result: configuration file found (${CUPSD_CONFIG_FILE})"
+            CUPSD_FOUND=1
+        else
+            Display --indent 2 --text "- Checking CUPS configuration file" --result "${STATUS_NOT_FOUND}" --color RED
+            LogText "Result: configuration file not found"
+            LogText "Development: no CUPS configuration file found"
+        fi
+    fi
+#
+#####</t>
+  </si>
+  <si>
+    <t>cupsd file perms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : PRNT-2307
+    # Description : Check CUPSd configuration file permissions
+    # TODO        : Add function
+    if [ ${CUPSD_FOUND} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no PRNT-2307 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check CUPSd configuration file permissions"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking CUPS configuration file permissions"
+        FIND=$(${LSBINARY} -l ${CUPSD_CONFIG_FILE} | ${CUTBINARY} -c 2-10)
+        LogText "Result: found ${FIND}"
+        if [ "${FIND}" = "r--------" -o "${FIND}" = "rw-------" -o "${FIND}" = "rw-r-----" -o "${FIND}" = "rw-rw----" ]; then
+            Display --indent 4 --text "- File permissions" --result "${STATUS_OK}" --color GREEN
+            AddHP 1 1
+        else
+            Display --indent 4 --text "- File permissions" --result "${STATUS_WARNING}" --color RED
+            ReportSuggestion ${TEST_NO} "Access to CUPS configuration could be more strict."
+            AddHP 1 2
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>cupsd daemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : PRNT-2308
+    # Description : Check CUPS daemon network configuration
+    if [ ${CUPSD_FOUND} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no PRNT-2308 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check CUPSd network configuration"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        FOUND=0
+        # Checking network addresses
+        LogText "Test: Checking CUPS daemon listening network addresses"
+        FIND=$(${GREPBINARY} "^Listen" ${CUPSD_CONFIG_FILE} | ${GREPBINARY} -v "/" | ${AWKBINARY} '{ print $2 }')
+        COUNT=0
+        for ITEM in ${FIND}; do
+            LogText "Found network address: ${ITEM}"
+            COUNT=$((COUNT + 1))
+            FOUND=1
+        done
+        # Check if daemon is only running on localhost
+        if [ ${FOUND} -eq 0 ]; then
+            LogText "Result: no listen statement found in CUPS configuration file"
+        elif [ ${COUNT} -eq 1 ]; then
+            if [ "${FIND}" = "localhost:631" -o "${FIND}" = "127.0.0.1:631" ]; then
+                LogText "Result: CUPS daemon only running on localhost"
+                AddHP 2 2
+            else
+                LogText "Result: CUPS daemon running on one or more interfaces (not limited to localhost)"
+                ReportSuggestion ${TEST_NO} "Check CUPS configuration if it really needs to listen on the network"
+                AddHP 1 2
+            fi
+        else
+            LogText "Result: CUPS daemon is running on several network addresses"
+            ReportSuggestion ${TEST_NO} "Check CUPS configuration if it really needs to run on several network addresses"
+            AddHP 1 2
+        fi
+        # Checking sockets
+        LogText "Test: Checking cups daemon listening sockets"
+        FIND=$(${GREPBINARY} "^Listen" ${CUPSD_CONFIG_FILE} | ${GREPBINARY} "/" | ${AWKBINARY} '{ print $2 }')
+        for ITEM in ${FIND}; do
+            LogText "Found socket address: ${ITEM}"
+            COUNT=$((COUNT + 1))
+        done
+        if [ ${COUNT} -eq 0 ]; then
+            Display --indent 2 --text "- Checking CUPS addresses/sockets" --result "${STATUS_NONE}" --color WHITE
+            LogText "Result: no addresses found on which CUPS daemon is listening"
+        else
+            Display --indent 2 --text "- Checking CUPS addresses/sockets" --result "${STATUS_FOUND}" --color GREEN
+            LogText "Result: CUPS daemon is listening on network/socket"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>lpd status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : PRNT-2314
+    # Description : Check lpd status
+    Register --test-no PRNT-2314 --weight L --network NO --category security --description "Check lpd status"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking lpd status"
+        IsRunning lpd
+        if [ ${RUNNING} -eq 1 ]; then
+            Display --indent 2 --text "- Checking lp daemon" --result "${STATUS_RUNNING}" --color GREEN
+            LogText "Result: lp daemon running"
+            LPD_RUNNING=1; PRINTING_DAEMON="lp"
+        else
+            Display --indent 2 --text "- Checking lp daemon" --result "${STATUS_NOT_RUNNING}" --color WHITE
+            LogText "Result: lp daemon not running"
+            AddHP 4 4
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>/etc/qconfig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : PRNT-2316
+    # Description : Check /etc/qconfig file
+    Register --test-no PRNT-2316 --os AIX --weight L --network NO --category security --description "Checking /etc/qconfig file"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking ${ROOTDIR}etc/qconfig"
+        QDAEMON_CONFIG_FILE="${ROOTDIR}etc/qconfig"
+        FileIsReadable ${QDAEMON_CONFIG_FILE}
+        if [ ${CANREAD} -eq 1 ]; then
+            FIND=$(${GREPBINARY} -v "^\*" ${QDAEMON_CONFIG_FILE} | ${EGREPBINARY} "backend|device")
+            if [ ! -z "${FIND}" ]; then
+                LogText "Result: printers are defined in ${QDAEMON_CONFIG_FILE}"
+                Display --indent 2 --text "- Checking /etc/qconfig file" --result "${STATUS_FOUND}" --color GREEN
+                QDAEMON_CONFIG_ENABLED=1
+            else
+                LogText "Result: ${QDAEMON_CONFIG_FILE} is empty. No printers are defined"
+                Display --indent 2 --text "- Checking /etc/qconfig file" --result EMPTY --color WHITE
+            fi
+        else
+            LogText "Result: Can not read ${QDAEMON_CONFIG_FILE} (no permission)"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>qdaemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : PRNT-2418
+    # Description : Check qdaemon printer spooler status
+    Register --test-no PRNT-2418 --os AIX --weight L --network NO --category security --description "Checking qdaemon printer spooler status"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking qdaemon status"
+        IsRunning qdaemon
+        if [ ${RUNNING} -eq 1 ]; then
+            LogText "Result: qdaemon daemon running"
+            Display --indent 2 --text "- Checking qdaemon daemon" --result "${STATUS_RUNNING}" --color GREEN
+            QDAEMON_RUNNING=1; PRINTING_DAEMON="qdaemon"
+        else
+            if [ ${QDAEMON_CONFIG_ENABLED} -eq 1 ]; then
+                LogText "Result: qdaemon daemon not running"
+                Display --indent 2 --text "- Checking qdaemon daemon" --result "${STATUS_NOT_RUNNING}" --color RED
+                ReportSuggestion ${TEST_NO} "Activate print spooler daemon (qdaemon) in order to process print jobs"
+            else
+                LogText "Result: qdaemon daemon not running"
+                Display --indent 2 --text "- Checking qdaemon daemon" --result "${STATUS_NOT_RUNNING}" --color WHITE
+            fi
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>old print jobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : PRNT-2420
+    # Description : Checking old print jobs
+    Register --test-no PRNT-2420 --os AIX --weight L --network NO --category security --description "Checking old print jobs"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking old print jobs"
+        DirectoryExists ${ROOTDIR}var/spool/lpd/qdir
+        if [ ${DIRECTORY_FOUND} -eq 1 ]; then
+            FIND=$(find ${ROOTDIR}var/spool/lpd/qdir -type f -mtime +1 2&gt; /dev/null | ${SEDBINARY} 's/ /!space!/g')
+            if HasData "${FIND}"; then
+                COUNT=0
+                for ITEM in ${FIND}; do
+                    FILE=$(echo ${ITEM} | ${SEDBINARY} 's/!space!/ /g')
+                    LogText "Found old print job: ${FILE}"
+                    COUNT=$((COUNT + 1))
+                done
+                LogText "Result: Found ${COUNT} old print jobs in /var/spool/lpd/qdir"
+                Display --indent 4 --text "- Checking old print jobs" --result "${STATUS_FOUND}" --color YELLOW
+                ReportSuggestion ${TEST_NO} "Check old print jobs in /var/spool/lpd/qdir to prevent new jobs from being processed"
+                LogText "Risk: Failed or defunct print jobs can occupy a lot of space and in some cases, prevent new jobs from being processed"
+            else
+                LogText "Result: Old print jobs not found in /var/spool/lpd/qdir"
+                Display --indent 4 --text "- Checking old print jobs" --result "${STATUS_NONE}" --color GREEN
+            fi
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>cron daemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SCHD-7702
+    # Description : Check cron daemon
+    Register --test-no SCHD-7702 --weight L --network NO --category security --description "Check status of cron daemon"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        FIND=$(${PSBINARY} aux | ${EGREPBINARY} "( cron$|/cron(d)? )")
+        if IsEmpty "${FIND}"; then
+            LogText "Result: no cron daemon found"
+            AddHP 3 3
+        else
+            LogText "Result: cron daemon running"
+            CROND_RUNNING=1
+            Report "crond_running=1"
+            Report "scheduler[]=crond"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>crontab / cronjobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SCHD-7704
+    # Description : Check crontab / cronjobs
+    Register --test-no SCHD-7704 --weight L --network NO --category security --description "Check crontab/cronjobs"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        BAD_FILE_PERMISSIONS=0
+        BAD_FILE_OWNERSHIP=0
+        FindCronJob() {
+            sCRONJOBS=$(${EGREPBINARY} '^([0-9*])' $1 | ${TRBINARY} '\t' ' ' | ${TRBINARY} -s ' ' | ${TRBINARY} ' ' ',' | ${SORTBINARY})
+        }
+        CRONTAB_FILE="${ROOTDIR}etc/crontab"
+        if [ -f ${CRONTAB_FILE} ]; then
+            if IsWorldWritable ${CRONTAB_FILE}; then LogText "Result: insecure file permissions for cronjob file ${CRONTAB_FILE}"; Report "insecure_fileperms_cronjob[]=${CRONTAB_FILE}"; BAD_FILE_PERMISSIONS=1; AddHP 0 5; fi
+            if ! IsOwnedByRoot ${CRONTAB_FILE}; then LogText "Result: incorrect owner found for cronjob file ${CRONTAB_FILE}"; Report "bad_fileowner_cronjob[]=${CRONTAB_FILE}"; BAD_FILE_OWNERSHIP=1; AddHP 0 5; fi
+            FindCronJob ${CRONTAB_FILE}
+            for ITEM in ${sCRONJOBS}; do
+                LogText "Found cronjob (${CRONTAB_FILE}): ${ITEM}"
+                Report "cronjob[]=${ITEM}"
+            done
+        fi
+        CRON_DIRS="${ROOTDIR}etc/cron.d"
+        for DIR in ${CRON_DIRS}; do
+            LogText "Test: checking directory ${DIR}"
+            if [ -d ${DIR} ]; then
+                if FileIsReadable ${DIR}; then
+                    LogText "Result: found directory ${DIR}"
+                    LogText "Test: searching files in ${DIR}"
+                    FIND=$(${FINDBINARY} ${DIR} -type f -print | ${GREPBINARY} -v ".placeholder")
+                    if IsEmpty "${FIND}"; then
+                        LogText "Result: no files found in ${DIR}"
+                    else
+                        LogText "Result: found one or more files in ${DIR}. Analyzing files.."
+                        for FILE in ${FIND}; do
+                            if IsWorldWritable ${FILE}; then LogText "Result: insecure file permissions for cronjob file ${J}"; Report "insecure_fileperms_cronjob[]=${J}"; BAD_FILE_PERMISSIONS=1; AddHP 0 5; fi
+                            if ! IsOwnedByRoot ${FILE}; then LogText "Result: incorrect owner found for cronjob file ${J}"; Report "bad_fileowner_cronjob[]=${J}"; BAD_FILE_OWNERSHIP=1; AddHP 0 5; fi
+                            FindCronJob ${FILE}
+                            if HasData "${sCRONJOBS}"; then
+                                for K in ${sCRONJOBS}; do
+                                    LogText "Result: Found cronjob (${FILE}): ${K}"
+                                    Report "cronjob[]=${FILE}"
+                                done
+                            fi
+                        done
+                        LogText "Result: done with analyzing files in ${DIR}"
+                    fi
+                else
+                    LogText "Result: can not read file or directory ${DIR}"
+                fi
+            else
+                LogText "Result: directory ${DIR} does not exist"
+            fi
+        done
+        CRON_DIRS="${ROOTDIR}etc/cron.hourly ${ROOTDIR}etc/cron.daily ${ROOTDIR}etc/cron.weekly ${ROOTDIR}etc/cron.monthly"
+        for I in ${CRON_DIRS}; do
+            LogText "Test: checking directory ${I}"
+            if [ -d ${I} ]; then
+                LogText "Result: found directory ${I}"
+                if FileIsReadable ${I}; then
+                    LogText "Test: searching files in ${I}"
+                    FIND=$(${FINDBINARY} ${I} -type f -print 2&gt; /dev/null | ${GREPBINARY} -v ".placeholder")
+                    if [ -z "${FIND}" ]; then
+                        LogText "Result: no files found in ${I}"
+                    else
+                        LogText "Result: found one or more files in ${I}. Analyzing files.."
+                        for J in ${FIND}; do
+                            if IsWorldWritable ${J}; then LogText "Result: insecure file permissions for cronjob file ${J}"; Report "insecure_fileperms_cronjob[]=${J}"; BAD_FILE_PERMISSIONS=1; AddHP 0 5; fi
+                            if ! IsOwnedByRoot ${J}; then LogText "Result: incorrect owner found for cronjob file ${J}"; Report "bad_fileowner_cronjob[]=${J}"; BAD_FILE_OWNERSHIP=1; AddHP 0 5; fi
+                            LogText "Result: Found cronjob (${I}): ${J}"
+                            Report "cronjob[]=${J}"
+                        done
+                        LogText "Result: done with analyzing files in ${I}"
+                    fi
+                else
+                    LogText "Result: directory permissions are too strict to enter it (which might be good)"
+                fi
+            else
+                LogText "Result: directory ${I} does not exist"
+            fi
+        done
+        # /var/spool/cron/* and /var/spool/cron/crontabs/*
+        # Search only in one tree, to avoid searching the tree twice
+        if [ -d /var/spool/cron/crontabs ]; then
+            FIND=$(${FINDBINARY} /var/spool/cron/crontabs -xdev -type f -print 2&gt; /dev/null)
+            for I in ${FIND}; do
+                if FileIsReadable ${I}; then
+                    FindCronJob ${I}
+                    for J in ${sCRONJOBS}; do
+                        LogText "Found cronjob (/var/spool/cron/crontabs): ${I} (${J})"
+                        Report "cronjob[]=${I}"
+                    done
+                fi
+            done
+        else
+            if [ -d /var/spool/cron ]; then
+                FIND=$(find /var/spool/cron -type f -print)
+                for I in ${FIND}; do
+                    if FileIsReadable ${I}; then
+                        FindCronJob ${I}
+                        for J in ${sCRONJOBS}; do
+                            LogText "Found cronjob (/var/spool/cron): ${I} (${J})"
+                            LogText "cronjob[]=${I}"
+                        done
+                    fi
+                done
+            fi
+        fi
+        # Anacron
+        if [ "${OS}" = "Linux" ]; then
+            if [ -f /etc/anacrontab ]; then
+                LogText "Test: checking anacrontab"
+                sANACRONJOBS=$(${EGREPBINARY} '^([0-9@])' /etc/anacrontab | ${TRBINARY} '\t' ' ' | ${TRBINARY} -s ' ' | ${TRBINARY} ' ' ',' | ${SORTBINARY})
+                if [ ! -z "${sANACRONJOBS}" ]; then
+                    Report "scheduler[]=anacron"
+                    for I in ${sANACRONJOBS}; do
+                        LogText "Found anacron job (/etc/anacrontab): ${I}"
+                        Report "cronjob[]=${I}"
+                    done
+                fi
+            fi
+        fi
+        # Show warning when an issue shows up. Even if *both* the permissions and ownership are wrong, just show one (prevent overload of warnings).
+        if [ ${BAD_FILE_PERMISSIONS} -eq 1 ]; then
+            ReportWarning "${TEST_NO}" "Found one or more cronjob files with incorrect file permissions (see log for details)"
+            Display --indent 2 --text "- Checking crontab/cronjob" --result "${STATUS_WARNING}" --color RED
+        elif [ ${BAD_FILE_OWNERSHIP} -eq 1 ]; then
+            ReportWarning "${TEST_NO}" "Found one or more cronjob files with incorrect ownership (see log for details)"
+            Display --indent 2 --text "- Checking crontab/cronjob" --result "${STATUS_WARNING}" --color RED
+        else
+            Display --indent 2 --text "- Checking crontab/cronjob" --result "${STATUS_DONE}" --color GREEN
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>atd status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SCHD-7718
+    # Description : Check atd status
+    Register --test-no SCHD-7718 --weight L --network NO --category security --description "Check at users"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking atd status"
+        FIND=$(${PSBINARY} ax | ${GREPBINARY} "/atd" | ${GREPBINARY} -v "grep")
+        if [ ! -z "${FIND}" ]; then
+            LogText "Result: at daemon active"
+            Display --indent 2 --text "- Checking atd status" --result "${STATUS_RUNNING}" --color GREEN
+            ATD_RUNNING=1
+            Report "scheduler[]=atd"
+        else
+            LogText "Result: at daemon not active"
+            if IsVerbose; then Display --indent 2 --text "- Checking atd status" --result "${STATUS_NOT_RUNNING}" --color WHITE; fi
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>at.users</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SCHD-7720
+    # Description : Check at users
+    # Notes       : if at.allow exists, only users listed can schedule at jobs
+    #               if at.allow does not exist, but at.deny does, everyone
+    #               except the listed ones can schedule jobs. If both can't be
+    #               found, only root can schedule jobs.
+    if [ ${ATD_RUNNING} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SCHD-7720 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check at users"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        AT_UNKNOWN=0
+        case ${OS} in
+            FreeBSD)          AT_ALLOW="${ROOTDIR}var/at/at.allow";        AT_DENY="${ROOTDIR}var/at/at.deny"         ;;
+            HPUX)             AT_ALLOW="${ROOTDIR}usr/lib/cron/at.allow";  AT_DENY="${ROOTDIR}usr/lib/cron/at.deny"   ;;
+            Linux)            AT_ALLOW="${ROOTDIR}etc/at.allow";           AT_DENY="${ROOTDIR}etc/at.deny"            ;;
+            OpenBSD)          AT_ALLOW="${ROOTDIR}var/cron/at.allow";      AT_DENY="${ROOTDIR}var/cron/at.deny"       ;;
+            SunOS)            AT_ALLOW="${ROOTDIR}etc/cron.d/at.allow";    AT_DENY="${ROOTDIR}etc/cron.d/at.deny"     ;;
+            *)                AT_UNKNOWN=1; LogText "Test skipped, files for at unknown"            ;;
+        esac
+        if [ ${AT_UNKNOWN} -eq 0 ]; then
+            LogText "Test: checking for file ${AT_ALLOW}"
+            if [ -f ${AT_ALLOW} ]; then
+                FileIsReadable ${AT_ALLOW}
+                if [ ${CANREAD} -eq 1 ]; then
+                    LogText "Result: file ${AT_ALLOW} exists, only listed users can schedule at jobs"
+                    FIND=$(${SORTBINARY} ${AT_ALLOW})
+                    if IsEmpty "${FIND}"; then
+                        LogText "Result: File empty, no users are allowed to schedule at jobs"
+                    else
+                        for ITEM in ${FIND}; do
+                           LogText "Allowed at user: ${ITEM}"
+                        done
+                    fi
+                else
+                    LogText "Result: can not read ${AT_ALLOW} (no permission)"
+                fi
+            else
+                LogText "Result: file ${AT_ALLOW} does not exist"
+                LogText "Test: checking for file ${AT_DENY}"
+                if [ -f ${AT_DENY} ]; then
+                    FileIsReadable ${AT_DENY}
+                    if [ ${CANREAD} -eq 1 ]; then
+                        LogText "Result: file ${AT_DENY} exists, only non listed users can schedule at jobs"
+                        FIND=$(${SORTBINARY} ${AT_DENY})
+                        if [ -z "${FIND}" ]; then
+                            LogText "Result: file is empty, no users are denied access to schedule jobs"
+                        else
+                            for ITEM in ${FIND}; do
+                                LogText "Denied at user: ${ITEM}"
+                            done
+                        fi
+                    else
+                        LogText "Result: can not read ${AT_DENY} (no permission)"
+                    fi
+                else
+                    LogText "Result: both ${AT_ALLOW} and ${AT_DENY} do not exist"
+                    LogText "Note: only root can schedule at jobs"
+                    AddHP 1 1
+                fi
+            fi
+            Display --indent 4 --text "- Checking at users" --result "${STATUS_DONE}" --color GREEN
+        else
+            Display --indent 4 --text "- Checking at users" --result "${STATUS_SKIPPED}" --color YELLOW
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>scheduled at jobs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SCHD-7724
+    # Description : Check scheduled at jobs
+    if [ ${ATD_RUNNING} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SCHD-7724 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check at jobs"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Check scheduled at jobs"
+        FIND=$(atq | ${GREPBINARY} -v "no files in queue" | ${AWKBINARY} '{gsub("\t"," ");print}' | ${SEDBINARY} 's/ /!space!/g')
+        if HasData "${FIND}"; then
+            LogText "Result: found one or more jobs"
+            for ITEM in ${FIND}; do
+                VALUE=$(echo ${ITEM} | ${SEDBINARY} 's/!space!/ /g')
+                LogText "Found at job: ${VALUE}"
+            done
+            Display --indent 4 --text "- Checking at jobs" --result "${STATUS_FOUND}" --color GREEN
+        else
+            LogText "Result: no pending at jobs"
+            Display --indent 4 --text "- Checking at jobs" --result "${STATUS_NONE}" --color GREEN
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>TTYs that can enter single user mode without pass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SHLL-6202
+    # Description : check all console TTYs in which root user can enter single user mode without password
+    Register --test-no SHLL-6202 --os FreeBSD --weight L --network NO --category security --description "Check console TTYs"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking console TTYs"
+        FIND=$(${EGREPBINARY} '^console' ${ROOTDIR}etc/ttys | ${GREPBINARY} -v 'insecure')
+        if [ -z "${FIND}" ]; then
+            Display --indent 2 --text "- Checking console TTYs" --result "${STATUS_OK}" --color GREEN
+            LogText "Result: console is secured against single user mode without password."
+        else
+            Display --indent 2 --text "- Checking console TTYs" --result "${STATUS_WARNING}" --color RED
+            LogText "Result: Found insecure console in ${ROOTDIR}etc/ttys. Single user mode login without password allowed!"
+            LogText "Output ${ROOTDIR}etc/ttys:"
+            LogText "${FIND}"
+            ReportWarning ${TEST_NO} "Found unprotected console in ${ROOTDIR}etc/ttys"
+            LogText "Possible solution: Change the console line from 'secure' to 'insecure'."
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /etc/shells available</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SHLL-6211
+    # Description : which shells are available according /etc/shells
+    Register --test-no SHLL-6211 --weight L --network NO --category security --description "Checking available and valid shells"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Searching for ${ROOTDIR}etc/shells"
+        if [ -f ${ROOTDIR}etc/shells ]; then
+            LogText "Result: Found ${ROOTDIR}etc/shells file"
+            LogText "Test: Reading available shells from ${ROOTDIR}etc/shells"
+            SSHELLS=$(${GREPBINARY} "^/" ${ROOTDIR}etc/shells)
+            CSSHELLS=0; CSSHELLS_ALL=0
+            Display --indent 2 --text "- Checking shells from ${ROOTDIR}etc/shells"
+            for I in ${SSHELLS}; do
+                CSSHELLS_ALL=$((CSSHELLS_ALL + 1))
+                Report "available_shell[]=${I}"
+                # TODO add check for symlinked shells
+                if [ -f ${I} ]; then
+                    LogText "Found installed shell: ${I}"
+                    CSSHELLS=$((CSSHELLS + 1))
+                else
+                    LogText "Shell ${I} not installed. Probably a dummy or non existing shell."
+                fi
+            done
+            Display --indent 4 --text "Result: found ${CSSHELLS_ALL} shells (valid shells: ${CSSHELLS})."
+        else
+            LogText "Result: ${ROOTDIR}etc/shells not found, skipping test"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>idle session killing tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SHLL-6220
+    # Description : check for idle session killing tools or settings
+    Register --test-no SHLL-6220 --weight L --network NO --category security --description "Checking available and valid shells"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        IDLE_TIMEOUT_METHOD=""
+        IDLE_TIMEOUT_READONLY=""
+        LogText "Test: Search for session timeout tools or settings in shell"
+        IsRunning timeoutd
+        if [ ${RUNNING} -eq 1 ]; then
+            IDLE_TIMEOUT=1
+            LogText "Result: found timeoutd process to kill idle sesions"
+            IDLE_TIMEOUT_METHOD="timeout-daemon"
+        fi
+        IsRunning autolog
+        if [ ${RUNNING} -eq 1 ]; then
+            IDLE_TIMEOUT=1
+            LogText "Result: found autolog process to kill idle sesions"
+            Report="session_timeout_method[]=autolog"
+            IDLE_TIMEOUT_METHOD="autolog"
+        fi
+        if [ -f ${ROOTDIR}etc/profile ]; then
+            # Determine if we can find a TMOUT value
+            FIND=$(${GREPBINARY} 'TMOUT=' ${ROOTDIR}etc/profile | ${TRBINARY} -d ' ' | ${TRBINARY} -d '\t' | ${GREPBINARY} -v "^#" | ${SEDBINARY} 's/export//' | ${SEDBINARY} 's/#.*//' | ${AWKBINARY} -F= '{ print $2 }')
+            # Determine if the value is exported (with export, readonly, or typeset)
+            FIND2=$(${GREPBINARY} '\(export\|readonly\|typeset -r\)[ \t]*TMOUT' ${ROOTDIR}etc/profile | ${GREPBINARY} -v "^#" | ${SEDBINARY} 's/#.*//' | ${AWKBINARY} '{ print $1 }')
+            if [ ! -z "${FIND}" ]; then
+                N=0; IDLE_TIMEOUT=1
+                for I in ${FIND}; do
+                    LogText "Output: ${I}"
+                    Report "session_timeout_value[]=${I}"
+                    N=$((N + 1))
+                done
+                if [ ${N} -eq 1 ]; then
+                    LogText "Result: found TMOUT value configured in ${ROOTDIR}etc/profile"
+                else
+                    LogText "Result: found several TMOUT values configured in ${ROOTDIR}etc/profile"
+                fi
+                IDLE_TIMEOUT_METHOD="profile"
+            else
+                LogText "Result: could not find TMOUT setting in ${ROOTDIR}etc/profile"
+            fi
+            if [ ! -z "${FIND2}" ]; then
+                N=0;
+                for I in ${FIND2}; do
+                    LogText "Output: ${I}"
+                    if [ "${I}" = "readonly" -o "${I}" = "typeset" ]; then
+                        N=$((N + 1))
+                    fi
+                done
+                if [ ${N} -gt 0 ]; then
+                    LogText "Result: found readonly setting in ${ROOTDIR}etc/profile (readonly or typeset -r)"
+                    IDLE_TIMEOUT_READONLY=1
+                else
+                    LogText "Result: NO readonly setting found in ${ROOTDIR}etc/profile (readonly or typeset -r)"
+                    IDLE_TIMEOUT_READONLY=0
+                fi
+            else
+                LogText "Result: could not find export, readonly or typeset -r in ${ROOTDIR}etc/profile"
+            fi
+        else
+            LogText "Result: skip ${ROOTDIR}etc/profile test, file not available on this system"
+        fi
+        if [ -d ${ROOTDIR}etc/profile.d ]; then
+            FIND=$(${LSBINARY} ${ROOTDIR}etc/profile.d/*.sh 2&gt; /dev/null)
+            if [ ! -z "${FIND}" ]; then
+                # Determine if we can find a TMOUT value
+                FIND=$(${FINDBINARY} ${ROOTDIR}etc/profile.d -name "*.sh" -type f -exec cat {} \; 2&gt; /dev/null | ${GREPBINARY} 'TMOUT=' | ${TRBINARY} -d ' ' | ${TRBINARY} -d '\t' | ${GREPBINARY} -v "^#" | ${SEDBINARY} 's/export//' | ${SEDBINARY} 's/#.*//' | ${AWKBINARY} -F= '{ print $2 }')
+                # Determine if the value is exported (with export, readonly, or typeset)
+                FIND2=$(${FINDBINARY} ${ROOTDIR}etc/profile.d -name "*.sh" -type f -exec cat {} \; 2&gt; /dev/null | ${GREPBINARY} '\(export\|readonly\|typeset -r\)[ \t]*TMOUT' | ${GREPBINARY} -v "^#" | ${SEDBINARY} 's/#.*//' | ${AWKBINARY} '{ print $1 }')
+                if [ ! -z "${FIND}" ]; then
+                    N=0; IDLE_TIMEOUT=1
+                    for I in ${FIND}; do
+                        LogText "Output: ${I}"
+                        Report "session_timeout_value[]=${I}"
+                        N=$((N + 1))
+                    done
+                    if [ ${N} -eq 1 ]; then
+                        LogText "Result: found TMOUT value configured in one of the files in ${ROOTDIR}etc/profile.d directory"
+                    else
+                        LogText "Result: found several TMOUT values configured in one of the files in ${ROOTDIR}etc/profile.d directory"
+                    fi
+                    IDLE_TIMEOUT_METHOD="profile.d"
+                else
+                    LogText "Result: could not find TMOUT setting in ${ROOTDIR}etc/profile.d/*.sh"
+                fi
+                # Check for readonly
+                if [ ! -z "${FIND2}" ]; then
+                    N=0;
+                    for I in ${FIND2}; do
+                        LogText "Output: ${I}"
+                        if [ "${I}" = "readonly" -o "${I}" = "typeset" ]; then
+                            N=$((N + 1))
+                        fi
+                    done
+                    if [ ${N} -gt 0 ]; then
+                        LogText "Result: found readonly setting in ${ROOTDIR}etc/profile (readonly or typeset -r)"
+                        IDLE_TIMEOUT_READONLY=1
+                    else
+                        LogText "Result: NO readonly setting found in ${ROOTDIR}etc/profile (readonly or typeset -r)"
+                        IDLE_TIMEOUT_READONLY=0
+                    fi
+                else
+                    LogText "Result: could not find export, readonly or typeset -r in ${ROOTDIR}etc/profile"
+                fi
+            fi
+        else
+            LogText "Result: skip ${ROOTDIR}etc/profile.d directory test, directory not available on this system"
+        fi
+        if [ ! -z "${IDLE_TIMEOUT_METHOD}" ]; then
+            Report "session_timeout_method[]=${IDLE_TIMEOUT_METHOD}"
+        fi
+        if [ ! -z "${IDLE_TIMEOUT_READONLY}" ]; then
+            Report "session_timeout_set_readonly=${IDLE_TIMEOUT_READONLY}"
+        fi
+        if [ ${IDLE_TIMEOUT} -eq 1 ]; then
+            Display --indent 4 --text "- Session timeout settings/tools" --result "${STATUS_FOUND}" --color GREEN
+            AddHP 3 3
+        else
+            Display --indent 4 --text "- Session timeout settings/tools" --result "${STATUS_NONE}" --color YELLOW
+            AddHP 1 3
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>umask values</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SHLL-6230
+    # Description : Check for umask values in shell configurations
+    SHELL_CONFIG_FILES="${ROOTDIR}etc/bashrc ${ROOTDIR}etc/bash.bashrc ${ROOTDIR}etc/csh.cshrc ${ROOTDIR}etc/profile"
+    Register --test-no SHLL-6230 --weight H --network NO --category security --description "Perform umask check for shell configurations"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        FOUND=0
+        HARDENING_POSSIBLE=0
+        Display --indent 2 --text "- Checking default umask values"
+        for FILE in ${SHELL_CONFIG_FILES}; do
+            FIND=""
+            if [ -f ${FILE} ]; then
+                LogText "Result: file ${FILE} exists"
+                FOUND=1
+                FIND=$(${GREPBINARY} umask ${FILE} | ${SEDBINARY} 's/^[ \t]*//g' | ${SEDBINARY} 's/#.*$//' | ${GREPBINARY} -v "^$" | ${AWKBINARY} '{ print $2 }')
+                if IsEmpty "${FIND}"; then
+                    LogText "Result: did not find umask configured in ${FILE}"
+                    Display --indent 4 --text "- Checking default umask in ${FILE}" --result "${STATUS_NONE}" --color YELLOW
+                else
+                    for UMASKVALUE in ${FIND}; do
+                        LogText "Result: found umask ${UMASKVALUE} in ${FILE}"
+                        case ${UMASKVALUE} in
+                            027|0027|077|0077)
+                                    LogText "Result: umask ${UMASKVALUE} is considered a properly hardened value"
+                            ;;
+                            *)
+                                    LogText "Result: umask ${UMASKVALUE} can be hardened "
+                                    HARDENING_POSSIBLE=1
+                            ;;
+                        esac
+                    done
+                    if [ ${HARDENING_POSSIBLE} -eq 0 ]; then
+                        Display --indent 4 --text "- Checking default umask in ${FILE}" --result "${STATUS_OK}" --color GREEN
+                        AddHP 3 3
+                    else
+                        Display --indent 4 --text "- Checking default umask in ${FILE}" --result WEAK --color YELLOW
+                        AddHP 1 3
+                    fi
+                fi
+            else
+                LogText "Result: file ${FILE} not found"
+            fi
+        done
+    fi
+#</t>
+  </si>
+  <si>
+    <t>snmp support</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    InsertSection "SNMP Support"
+    # Test        : SNMP-3302
+    # Description : Check for a running SNMP daemon
+    Register --test-no SNMP-3302 --weight L --network NO --category security --description "Check for running SNMP daemon"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Searching for a SNMP daemon"
+        # Check running processes
+        IsRunning snmpd
+        if [ ${RUNNING} -eq 1 ]; then
+            SNMP_DAEMON_RUNNING=1
+            LogText "Result: SNMP daemon is running"
+            Display --indent 2 --text "- Checking running SNMP daemon" --result "${STATUS_FOUND}" --color GREEN
+        else
+            LogText "Result: No running SNMP daemon found"
+            Display --indent 2 --text "- Checking running SNMP daemon" --result "${STATUS_NOT_FOUND}" --color WHITE
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>snmp daemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SNMP-3304
+    # Description : Determine SNMP daemon configuration file location
+    if [ ${SNMP_DAEMON_RUNNING} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SNMP-3304 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check SNMP daemon file location"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: searching for snmpd.conf file"
+        for I in ${SNMP_DAEMON_CONFIG_LOCS}; do
+            if [ -f "${I}/snmpd.conf" ]; then
+                LogText "Result: ${I}/snmpd.conf exists"
+                SNMP_DAEMON_CONFIG="${I}/snmpd.conf"
+            fi
+        done
+        if [ -z "${SNMP_DAEMON_CONFIG}" ]; then
+            LogText "Result: No snmpd configuration found"
+            Display --indent 4 --text "- Checking SNMP configuration" --result "${STATUS_NOT_FOUND}" --color WHITE
+        else
+            LogText "Result: using last found configuration file: ${SNMP_DAEMON_CONFIG}"
+            Display --indent 4 --text "- Checking SNMP configuration" --result "${STATUS_FOUND}" --color GREEN
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>snmp communities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SNMP-3306
+    # Description : Determine SNMP communities
+    if [ ! -z "${SNMP_DAEMON_CONFIG}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SNMP-3306 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check SNMP communities"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        WARN=0
+        LogText "Test: reading active snmp communities"
+        FIND=$(${AWKBINARY} '/^com2sec/ { print $4 }' ${SNMP_DAEMON_CONFIG})
+        for I in ${FIND}; do
+            LogText "Output: ${I}"
+            if [ "${I}" = "public" -o "${I}" = "private" ]; then
+                LogText "Result: found easy guessable snmp community string (${I})"
+                WARN=1
+                AddHP 1 3
+            fi
+        done
+        # Check status of test
+        if [ ${WARN} -eq 0 ]; then
+            Display --indent 2 --text "- Checking SNMP community strings" --result "${STATUS_OK}" --color GREEN
+            AddHP 2 2
+        else
+            Display --indent 2 --text "- Checking SNMP community strings" --result "${STATUS_WARNING}" --color RED
+            ReportWarning ${TEST_NO} "Found easy guessable SNMP community string"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>running squid daemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SQD-3602
+    # Description : Check for a running Squid daemon
+    # Notes       : Search for squid(3) with a space, to avoid SquidGuard and other
+    #               programs.
+    Register --test-no SQD-3602 --weight L --network NO --category security --description "Check for running Squid daemon"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Searching for a Squid daemon"
+        FOUND=0
+        # Check running processes
+        FIND=$(${PSBINARY} ax | ${EGREPBINARY} "(squid|squid3) " | ${GREPBINARY} -v "grep")
+        if [ ! -z "${FIND}" ]; then
+            SQUID_DAEMON_RUNNING=1
+            LogText "Result: Squid daemon is running"
+            Display --indent 2 --text "- Checking running Squid daemon" --result "${STATUS_FOUND}" --color GREEN
+        else
+            LogText "Result: No running Squid daemon found"
+            Display --indent 2 --text "- Checking running Squid daemon" --result "${STATUS_NOT_FOUND}" --color WHITE
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>squid daemon config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SQD-3604
+    # Description : Determine Squid daemon configuration file location
+    if [ ${SQUID_DAEMON_RUNNING} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SQD-3604 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check Squid daemon file location"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: searching for squid.conf or squid3.conf file"
+        for I in ${SQUID_DAEMON_CONFIG_LOCS}; do
+            # Checking squid.conf
+            if [ -f "${I}/squid.conf" ]; then
+                LogText "Result: ${I}/squid.conf exists"
+                SQUID_DAEMON_CONFIG="${I}/squid.conf"
+            fi
+            # Checking squid3.conf
+            if [ -f "${I}/squid3.conf" ]; then
+                LogText "Result: ${I}/squid3.conf exists"
+                SQUID_DAEMON_CONFIG="${I}/squid3.conf"
+            fi
+        done
+        if [ -z "${SQUID_DAEMON_CONFIG}" ]; then
+            LogText "Result: No Squid configuration file found"
+            Display --indent 4 --text "- Searching Squid configuration file" --result "${STATUS_NOT_FOUND}" --color YELLOW
+        else
+            LogText "Result: using last found configuration file: ${SQUID_DAEMON_CONFIG}"
+            Display --indent 4 --text "- Searching Squid configuration" --result "${STATUS_FOUND}" --color GREEN
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>squid version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SQD-3606
+    # Description : Check Squid version
+    if [ ${SQUID_DAEMON_RUNNING} -eq 1 -a ! -z "${SQUID_DAEMON_CONFIG}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SQD-3606 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check Squid version"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        if [ ! -z "${SQUIDBINARY}" ]; then
+            LogText "Result: Squid binary found (${SQUIDBINARY})"
+            # Skip check if a setuid/setgid bit is found
+            FIND=$(${FINDBINARY} ${SQUIDBINARY} \( -perm 4000 -o -perm 2000 \) -print)
+            if [ -z "${FIND}" ]; then
+                FIND2=$(${SQUIDBINARY} -v | ${AWKBINARY} '{ if ($3=="Version") { print $4 } }')
+                Display --indent 4 --text "- Checking Squid version" --result "${STATUS_FOUND}" --color GREEN
+                SQUID_VERSION="${FIND2}"
+            else
+                LogText "Result: test skipped for security reasons, setuid/setgid bit set"
+                Display --indent 4 --text "- Checking Squid version" --result "${STATUS_SKIPPED}" --color RED
+            fi
+        else
+            LogText "Result: no Squid binary found"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>squid config options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SQD-3610
+    # Description : Check Squid configuration options
+    if [ ${SQUID_DAEMON_RUNNING} -eq 1 -a ! -z "${SQUID_DAEMON_CONFIG}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SQD-3610 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check Squid version"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking all specific defined options in ${SQUID_DAEMON_CONFIG}"
+        FIND=$(${GREPBINARY} -v "^#" ${SQUID_DAEMON_CONFIG} | ${GREPBINARY} -v "^$" | ${AWKBINARY} '{gsub("\t"," ");print}' | ${SEDBINARY} 's/ /!space!/g')
+        for I in ${FIND}; do
+            I=$(echo ${I} | ${SEDBINARY} 's/!space!/ /g')
+            LogText "Found Squid option: ${I}"
+            Report "squid_option=${I}"
+        done
+        Display --indent 4 --text "- Checking defined Squid options" --result "${STATUS_DONE}" --color GREEN
+    fi
+#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SQD-3613
+    # Description : Check Squid configuration options
+    if [ ${SQUID_DAEMON_RUNNING} -eq 1 -a ! -z "${SQUID_DAEMON_CONFIG}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SQD-3613 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check Squid file permissions"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking file permissions of ${SQUID_DAEMON_CONFIG}"
+        FIND=$(find ${SQUID_DAEMON_CONFIG} -type f -a \( -perm -004 -o -perm -002 -o -perm -001 \))
+        if [ ! -z "${FIND}" ]; then
+            LogText "Result: file ${SQUID_DAEMON_CONFIG} is world readable, writable or executable and could leak information or passwords"
+            Display --indent 4 --text "- Checking Squid configuration file permissions" --result "${STATUS_WARNING}" --color RED
+            ReportSuggestion ${TEST_NO} "Check file permissions of ${SQUID_DAEMON_CONFIG} to limit access"
+            ReportWarning ${TEST_NO} "File permissions of ${SQUID_DAEMON_CONFIG} are not restrictive"
+            AddHP 0 2
+        else
+            LogText "Result: file ${SQUID_DAEMON_CONFIG} has proper file permissions"
+            Display --indent 4 --text "- Checking Squid configuration file permissions" --result "${STATUS_OK}" --color GREEN
+            AddHP 2 2
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>squid auth</t>
+  </si>
+  <si>
+    <t>#
+    # Test        : SQD-3614
+    # Description : Check Squid authentication
+    if [ ${SQUID_DAEMON_RUNNING} -eq 1 -a ! -z "${SQUID_DAEMON_CONFIG}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SQD-3614 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check Squid authentication methods"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: check auth_param option for authentication methods"
+        FIND=$(${GREPBINARY} "^auth_param" ${SQUID_DAEMON_CONFIG} | ${AWKBINARY} '{ print $2 }')
+        if [ -z "${FIND}" ]; then
+            LogText "No auth_param option found, proxy access anonymous or based on other methods (like ACLs)"
+            Display --indent 6 --text "- Checking Squid authentication methods" --result "${STATUS_NONE}" --color YELLOW
+        else
+            Display --indent 6 --text "- Checking Squid authentication methods" --result "${STATUS_FOUND}" --color GREEN
+            for I in ${FIND}; do
+                LogText "Result: found authentication method ${I}"
+                Report "squid_auth_method=${I}"
+            done
+        fi
+    fi</t>
+  </si>
+  <si>
+    <t>squid authentication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SQD-3616
+    # Description : Check external Squid authentication
+    if [ ${SQUID_DAEMON_RUNNING} -eq 1 -a ! -z "${SQUID_DAEMON_CONFIG}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SQD-3616 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check external Squid authentication"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: check external_acl_type option for external authentication helpers"
+        FIND=$(${GREPBINARY} "^external_acl_type" ${SQUID_DAEMON_CONFIG})
+        if [ -z "${FIND}" ]; then
+            LogText "No external_acl_type found"
+            Display --indent 6 --text "- Checking Squid external authentication methods" --result "${STATUS_NONE}" --color YELLOW
+        else
+            Display --indent 6 --text "- Checking Squid external authentication methods" --result "${STATUS_FOUND}" --color GREEN
+            for I in ${FIND}; do
+                LogText "Result: found external authentication method helper"
+                LogText "Output: ${FIND}"
+                #Report "squid_external_acl_type=TRUE"
+            done
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>check ACLs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SQD-3620
+    # Description : Check ACLs
+    if [ ${SQUID_DAEMON_RUNNING} -eq 1 -a ! "${SQUID_DAEMON_CONFIG}" = "" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SQD-3620 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check Squid access control lists"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        COUNT=0
+        LogText "Test: checking ACLs"
+        FIND=$(${GREPBINARY} "^acl " ${SQUID_DAEMON_CONFIG} | ${SEDBINARY} 's/ /!space!/g')
+        if [ "${FIND}" = "" ]; then
+            LogText "Result: No ACLs found"
+            Display --indent 6 --text "- Checking Access Control Lists" --result "${STATUS_NONE}" --color RED
+        else
+            for ITEM in ${FIND}; do
+                COUNT=$((COUNT + 1))
+                ITEM=$(echo ${ITEM} | ${SEDBINARY} 's/!space!/ /g')
+                LogText "Found ACL: ${ITEM}"
+                #Report "squid_acl=${ITEM}" # TODO
+            done
+            LogText "Result: Found ${COUNT} ACLs"
+            Display --indent 6 --text "- Checking Access Control Lists" --result "${COUNT} ACLs FOUND" --color GREEN
+        fi
+    fi</t>
+  </si>
+  <si>
+    <t>unsecure ports in Safe_ports list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SQD-3624
+    # Description : Check unsecure ports in Safe_ports list
+    if [ ${SQUID_DAEMON_RUNNING} -eq 1 -a ! "${SQUID_DAEMON_CONFIG}" = "" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SQD-3624 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check Squid safe ports"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: checking ACL Safe_ports http_access option"
+        FIND=$(${GREPBINARY} "^http_access" ${SQUID_DAEMON_CONFIG} | ${GREPBINARY} "Safe_ports")
+        if IsEmpty "${FIND}"; then
+            LogText "Result: no Safe_ports found"
+            Display --indent 6 --text "- Checking ACL 'Safe_ports' http_access option" --result "${STATUS_NOT_FOUND}" --color YELLOW
+            ReportSuggestion ${TEST_NO} "Check if Squid has been configured to restrict access to all safe ports"
+        else
+            LogText "Result: checking ACL safe ports"
+            FIND2=$(${GREPBINARY} "^acl Safe_ports port" ${SQUID_DAEMON_CONFIG} | ${AWKBINARY} '{ print $4 }')
+            if IsEmpty "${FIND2}"; then
+                Display --indent 6 --text "- Checking ACL 'Safe_ports' ports" --result "NONE FOUND" --color YELLOW
+                ReportSuggestion ${TEST_NO} "Check if Squid has been configured for which ports it can allow outgoing traffic (Safe_ports)"
+                AddHP 0 1
+            else
+                LogText "Result: Safe_ports found"
+                for ITEM in ${FIND}; do
+                    LogText "Found safe port: ${ITEM}"
+                done
+                Display --indent 6 --text "- Checking ACL 'Safe_ports' ports" --result "${STATUS_FOUND}" --color GREEN
+                AddHP 1 1
+            fi
+            for ITEM in ${SQUID_DAEMON_UNSAFE_PORTS_LIST}; do
+                LogText "Test: Checking port ${ITEM} in Safe_ports list"
+                FIND2=$(${GREPBINARY} -w "^acl Safe_ports port ${ITEM}" ${SQUID_DAEMON_CONFIG})
+                if IsEmpty "${FIND2}"; then
+                    Display --indent 6 --text "- Checking ACL 'Safe_ports' (port ${ITEM})" --result "${STATUS_NOT_FOUND}" --color GREEN
+                    AddHP 1 1
+                else
+                    Display --indent 6 --text "- Checking ACL 'Safe_ports' (port ${ITEM})" --result "${STATUS_FOUND}" --color RED
+                    ReportWarning ${TEST_NO} "Squid configuration possibly allows relaying traffic via configured Safe_port ${ITEM}"
+                    AddHP 0 1
+                fi
+            done
+        fi
+    fi</t>
+  </si>
+  <si>
+    <t>reply_body_max_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SQD-3630 [T]
+    # Description : Check reply_body_max_size value
+    if [ ${SQUID_DAEMON_RUNNING} -eq 1 -a ! -z "${SQUID_DAEMON_CONFIG}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SQD-3630 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check Squid reply_body_max_size option"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: checking option reply_body_max_size"
+        FIND=$(${GREPBINARY} "^reply_body_max_size " ${SQUID_DAEMON_CONFIG} | ${SEDBINARY} 's/ /!space!/g')
+        if IsEmpty "${FIND}"; then
+            LogText "Result: option reply_body_max_size not configured"
+            Display --indent 6 --text "- Checking option: reply_body_max_size" --result "${STATUS_NONE}" --color RED
+            AddHP 1 2
+            ReportSuggestion ${TEST_NO} "Configure Squid option reply_body_max_size to limit the upper size of requests."
+        else
+            LogText "Result: option reply_body_max_size configured"
+            LogText "Output: ${FIND}"
+            Display --indent 6 --text "- Checking option: reply_body_max_size" --result "${STATUS_FOUND}" --color GREEN
+            AddHP 2 2
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>httpd_suppress_version_string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SQD-3680
+    # Description : Check httpd_suppress_version_string
+    if [ ${SQUID_DAEMON_RUNNING} -eq 1 -a ! -z "${SQUID_DAEMON_CONFIG}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SQD-3680 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check Squid version suppresion"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        FIND=$(${GREPBINARY} "^httpd_suppress_version_string " ${SQUID_DAEMON_CONFIG} | ${GREPBINARY} " on")
+        if [ -z "${FIND}" ]; then
+            LogText "Result: option httpd_suppress_version_string not configured"
+            Display --indent 6 --text "- Checking option: httpd_suppress_version_string" --result "${STATUS_NOT_FOUND}" --color YELLOW
+            AddHP 1 2
+            ReportSuggestion ${TEST_NO} "Configure Squid option httpd_suppress_version_string (on) to suppress the version."
+        else
+            LogText "Result: option httpd_suppress_version_string configured"
+            LogText "Output: ${FIND}"
+            Display --indent 6 --text "- Checking option: httpd_suppress_version_string" --result "${STATUS_FOUND}" --color GREEN
+            AddHP 2 2
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>ssh daemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SSH-7402
+    # Description : Check for a running SSH daemon
+    Register --test-no SSH-7402 --weight L --network NO --category security --description "Check for running SSH daemon"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Searching for a SSH daemon"
+        IsRunning sshd
+        if [ ${RUNNING} -eq 1 ] || PortIsListening "TCP" 22; then
+            SSH_DAEMON_RUNNING=1
+            Display --indent 2 --text "- Checking running SSH daemon" --result "${STATUS_FOUND}" --color GREEN
+            # Store settings in a temporary file
+            CreateTempFile
+            SSH_DAEMON_OPTIONS_FILE="${TEMP_FILE}"
+            ${SSHDBINARY} -T 2&gt; /dev/null &gt; ${SSH_DAEMON_OPTIONS_FILE}
+        else
+            Display --indent 2 --text "- Checking running SSH daemon" --result "${STATUS_NOT_FOUND}" --color WHITE
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>ssh daemon config file location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SSH-7404
+    # Description : Determine SSH daemon configuration file location
+    if [ ${SSH_DAEMON_RUNNING} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SSH-7404 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check SSH daemon file location"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        FOUND=0
+        LogText "Test: searching for sshd_config file"
+        for I in ${SSH_DAEMON_CONFIG_LOCS}; do
+            if [ -f "${I}/sshd_config" ]; then
+                LogText "Result: ${I}/sshd_config exists"
+                if [ ${FOUND} -eq 1 ]; then
+                    ReportException "${TEST_NO}:01"
+                    LogText "Result: we already had found another sshd_config file. Using this new file then."
+                fi
+                FileIsReadable ${I}/sshd_config
+                if [ ${CANREAD} -eq 1 ]; then
+                    FOUND=1
+                    SSH_DAEMON_CONFIG="${I}/sshd_config"
+                else
+                    LogText "Result: can not read ${I}/sshd_config file (no permission)"
+                fi
+            fi
+        done
+        if [ -z "${SSH_DAEMON_CONFIG}" ]; then
+            LogText "Result: No sshd configuration found"
+            Display --indent 4 --text "- Searching SSH configuration" --result "${STATUS_NOT_FOUND}" --color YELLOW
+            ReportException "${TEST_NO}:1" "SSH daemon is running, but no readable configuration file found"
+        else
+            LogText "Result: using last found configuration file: ${SSH_DAEMON_CONFIG}"
+            Display --indent 4 --text "- Searching SSH configuration" --result "${STATUS_FOUND}" --color GREEN
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>Check specific ssh options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SSH-7408
+    # Description : Check SSH specific defined options
+    # Notes       : Instead of parsing the configuration file, we query the SSH daemon itself
+    if [ ${SSH_DAEMON_RUNNING} -eq 1 -a ! -z "${SSH_DAEMON_OPTIONS_FILE}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SSH-7408 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check SSH specific defined options"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking specific defined options in ${SSH_DAEMON_OPTIONS_FILE}"
+        ## SSHOPTIONS scheme:
+        ##      &lt;OptionName&gt;:&lt;ExpectedValue&gt;,&lt;MediumScoreValue&gt;,&lt;WeakValue&gt;:&lt;TestType&gt;
+        ##
+        ##      Test types:
+        ##      (a) '='         -- equal to is better,
+        ##      (b) '&lt;'         -- less or equal is better,
+        ##      (c) '&gt;'         -- more or equal is better,
+        ##      (d) '!'         -- not equal is better.
+        ##
+        ##      Example:
+        ##      PermitRootLogin:NO,WITHOUT-PASSWORD,YES,:=
+        SSHOPS="AllowTcpForwarding:NO,LOCAL,YES:=\
+                ClientAliveCountMax:2,4,16:&lt;\
+                ClientAliveInterval:300,600,900:&lt;\
+                Compression:(DELAYED|NO),,YES:=\
+                FingerprintHash:SHA256,MD5,:=\
+                GatewayPorts:NO,,YES:=\
+                IgnoreRhosts:YES,,NO:=\
+                LoginGraceTime:120,240,480:&lt;\
+                LogLevel:VERBOSE,INFO,:=\
+                MaxAuthTries:2,4,6:&lt;\
+                MaxSessions:2,4,8:&lt;\
+                PermitRootLogin:NO,(PROHIBIT-PASSWORD|WITHOUT-PASSWORD),YES:=\
+                PermitUserEnvironment:NO,,YES:=\
+                PermitTunnel:NO,,YES:=\
+                Port:,,22:!\
+                PrintLastLog:YES,,NO:=\
+                Protocol:2,,1:=\
+                StrictModes:YES,,NO:=\
+                TCPKeepAlive:NO,,YES:=\
+                UseDNS:NO,,YES:=\
+                UsePrivilegeSeparation:SANDBOX,YES,NO:=\
+                VerifyReverseMapping:YES,,NO:=\
+                X11Forwarding:NO,,YES:=\
+                AllowAgentForwarding:NO,,YES:="
+        # Notes
+        # =========================================================
+        # UsePrivilegeSeparation - removed since OpenSSH 7.5
+        #
+        # Disabled        MaxStartups:4,8,16:&lt;\ (needs fixing)
+        # Go through our list of options
+        for I in ${SSHOPS}; do
+            OPTIONNAME=$(echo ${I} | ${CUTBINARY} -d ':' -f1)
+            OPTIONNAME_LOWER=$(echo ${I} | ${CUTBINARY} -d ':' -f1 | ${AWKBINARY} '{ print tolower($1) }')
+            EXPECTEDVALUE=$(echo ${I} | ${CUTBINARY} -d ':' -f2 | ${CUTBINARY} -d',' -f1)
+            MEDIUMSCOREDVALUE=$(echo ${I} | ${CUTBINARY} -d ':' -f2 | ${CUTBINARY} -d',' -f2)
+            WEAKVALUE=$(echo ${I} | ${CUTBINARY} -d ':' -f2 | ${CUTBINARY} -d',' -f3)
+            TESTTYPE=$(echo ${I} | ${CUTBINARY} -d ':' -f3)
+            RESULT="NONE"
+            if ! SkipAtomicTest "${TEST_NO}:${OPTIONNAME_LOWER}"; then
+                # Get value and use the last occurrence
+                FOUNDVALUE=$(${AWKBINARY} -v OPT="${OPTIONNAME_LOWER}" 'index($0, OPT) == 1 { print toupper($2) }' ${SSH_DAEMON_OPTIONS_FILE} | tail -1)
+                LogText "Test: Checking ${OPTIONNAME} in ${SSH_DAEMON_OPTIONS_FILE}"
+                if [ ! -z "${FOUNDVALUE}" ]; then
+                    LogText "Result: Option ${OPTIONNAME} found"
+                    LogText "Result: Option ${OPTIONNAME} value is ${FOUNDVALUE}"
+                    if [ "${TESTTYPE}" = "=" ]; then
+                        if [ "${FOUNDVALUE}" = "${EXPECTEDVALUE}" ]; then
+                            RESULT="GOOD"
+                        elif [ "${FOUNDVALUE}" = "${MEDIUMSCOREDVALUE}" ]; then
+                            RESULT="MIDSCORED"
+                        elif [ "${FOUNDVALUE}" = "${WEAKVALUE}" ]; then
+                            RESULT="WEAK"
+                        else
+                            if [ ! -z "${EXPECTEDVALUE}" ]; then
+                                LogText "Expected value has multiple values, testing if active value is in list (${EXPECTEDVALUE})"
+                                FIND=$(echo ${FOUNDVALUE} | ${GREPBINARY} -E "${EXPECTEDVALUE}")
+                                if [ $? -eq 0 ]; then
+                                    LogText "Result: found"
+                                    RESULT="GOOD"
+                                else
+                                    LogText "Result: not found"
+                                fi
+                            fi
+                            if [ ! -z "${MEDIUMSCOREDVALUE}" ]; then
+                                LogText "Medium scored value has multiple values, testing if active value is in list (${MEDIUMSCOREDVALUE})"
+                                FIND=$(echo ${FOUNDVALUE} | ${GREPBINARY} -E "${MEDIUMSCOREDVALUE}")
+                                if [ $? -eq 0 ]; then
+                                    LogText "Result: found"
+                                    RESULT="MIDSCORED"
+                                else
+                                    LogText "Result: not found"
+                                fi
+                            fi
+                            # Set result to weak if we can't find any matches
+                            if [ "${RESULT}" = "NONE" ]; then RESULT="WEAK"; fi
+                        fi
+                    elif [ "${TESTTYPE}" = "&lt;" ]; then
+                        if [ "${FOUNDVALUE}" -ge "${WEAKVALUE}" -o "${FOUNDVALUE}" -gt "${MEDIUMSCOREDVALUE}" ]; then
+                            RESULT="WEAK"
+                        elif [ "${FOUNDVALUE}" -le "${MEDIUMSCOREDVALUE}" -a "${FOUNDVALUE}" -gt "${EXPECTEDVALUE}" ]; then
+                            RESULT="MIDSCORED"
+                        elif [ "${FOUNDVALUE}" -le "${EXPECTEDVALUE}" ]; then
+                            RESULT="GOOD"
+                        else
+                            RESULT="UNKNOWN"
+                        fi
+                    elif [ "${TESTTYPE}" = "&gt;" ]; then
+                        if [ "${FOUNDVALUE}" -le "${WEAKVALUE}" ]; then
+                            RESULT="WEAK"
+                        elif [ "${FOUNDVALUE}" -le "${WEAKVALUE}" -a "${FOUNDVALUE}" -ge "${MEDIUMSCOREDVALUE}" ]; then
+                            RESULT="MIDSCORED"
+                        elif [ "${FOUNDVALUE}" -ge "${EXPECTEDVALUE}" ]; then
+                            RESULT="GOOD"
+                        else
+                            RESULT="UNKNOWN"
+                        fi
+                    elif [ "${TESTTYPE}" = "!" ]; then
+                        if [ "${FOUNDVALUE}" = "${WEAKVALUE}" ]; then
+                            RESULT="WEAK"
+                        elif [ ! "${FOUNDVALUE}" = "${WEAKVALUE}" ]; then
+                            RESULT="GOOD"
+                        else
+                            RESULT="UNKNOWN"
+                        fi
+                    else
+                        RESULT="NONE"
+                    fi
+                fi
+                if [ "${RESULT}" = "GOOD" ]; then
+                    LogText "Result: SSH option ${OPTIONNAME} is configured very well"
+                    Display --indent 4 --text "- SSH option: ${OPTIONNAME}" --result "${STATUS_OK}" --color GREEN
+                    AddHP 3 3
+                elif [ "${RESULT}" = "MIDSCORED" ]; then
+                    LogText "Result: SSH option ${OPTIONNAME} is configured reasonably"
+                    ReportSuggestion ${TEST_NO} "Consider hardening SSH configuration" "${OPTIONNAME} (${FOUNDVALUE} --&gt; ${EXPECTEDVALUE})" "-"
+                    ReportDetails --test "${TEST_NO}" --service "sshd" --field "${OPTIONNAME}" --value "${FOUNDVALUE}" --preferredvalue "${EXPECTEDVALUE}" --description "sshd option ${OPTIONNAME}"
+                    Display --indent 4 --text "- SSH option: ${OPTIONNAME}" --result "${STATUS_SUGGESTION}" --color YELLOW
+                    AddHP 1 3
+                elif [ "${RESULT}" = "WEAK" ]; then
+                    LogText "Result: SSH option ${OPTIONNAME} is in a weak configuration state and should be fixed"
+                    ReportSuggestion ${TEST_NO} "Consider hardening SSH configuration" "${OPTIONNAME} (${FOUNDVALUE} --&gt; ${EXPECTEDVALUE})" "-"
+                    ReportDetails --test "${TEST_NO}" --service "sshd" --field "${OPTIONNAME}" --value "${FOUNDVALUE}" --preferredvalue "${EXPECTEDVALUE}" --description "sshd option ${OPTIONNAME}"
+                    Display --indent 4 --text "- SSH option: ${OPTIONNAME}" --result "${STATUS_SUGGESTION}" --color YELLOW
+                    AddHP 0 3
+                elif [ "${RESULT}" = "UNKNOWN" ]; then
+                    LogText "Result: Value of SSH option ${OPTIONNAME} is unknown (not defined)"
+                    Display --indent 4 --text "- SSH option: ${OPTIONNAME}" --result DEFAULT --color WHITE
+                    Report "unknown_config_option[]=ssh|$SSH_DAEMON_CONFIG}|${OPTIONNAME}|"
+                else
+                    LogText "Result: Option ${OPTIONNAME} not found in output"
+                    Display --indent 4 --text "- SSH option: ${OPTIONNAME}" --result "${STATUS_NOT_FOUND}" --color WHITE
+                fi
+            else
+                if IsVerbose; then Display --indent 4 --text "- SSH option: ${OPTIONNAME}" --result "SKIPPED (via config)" --color WHITE; fi
+            fi
+        done
+    fi
+#</t>
+  </si>
+  <si>
+    <t>allowed users/groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : SSH-7440
+    # Description : AllowUsers / AllowGroups
+    # Goal        : Check if only a specific amount of users/groups can log in to the system
+    if [ ${SSH_DAEMON_RUNNING} -eq 1 -a ! -z "${SSH_DAEMON_OPTIONS_FILE}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no SSH-7440 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check SSH option: AllowUsers and AllowGroups"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        FOUND=0
+        # AllowUsers
+        FIND=$(${EGREPBINARY} -i "^AllowUsers" ${SSH_DAEMON_OPTIONS_FILE} | ${AWKBINARY} '{ print $2 }')
+        if [ ! -z "${FIND}" ]; then
+            LogText "Result: AllowUsers set, with value ${FIND}"
+            Display --indent 4 --text "- SSH option: AllowUsers" --result "${STATUS_FOUND}" --color GREEN
+            FOUND=1
+        else
+            LogText "Result: AllowUsers is not set"
+            Display --indent 4 --text "- SSH option: AllowUsers" --result "${STATUS_NOT_FOUND}" --color WHITE
+        fi
+        # AllowGroups
+        FIND=$(${EGREPBINARY} -i "^AllowGroups" ${SSH_DAEMON_OPTIONS_FILE} | ${AWKBINARY} '{ print $2 }')
+        if [ ! -z "${FIND}" ]; then
+            LogText "Result: AllowUsers set ${FIND}"
+            Display --indent 4 --text "- SSH option: AllowGroups" --result "${STATUS_FOUND}" --color GREEN
+            FOUND=1
+        else
+            LogText "Result: AllowGroups is not set"
+            Display --indent 4 --text "- SSH option: AllowGroups" --result "${STATUS_NOT_FOUND}" --color WHITE
+        fi
+        if [ ${FOUND} -eq 1 ]; then
+            LogText "Result: SSH is limited to a specific set of users, which is good"
+            AddHP 2 2
+        else
+            LogText "Result: SSH has no specific user or group limitation. Most likely all valid users can SSH to this machine."
+            AddHP 0 1
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>disabled firewire storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1846
+    # Description : Check for disabled firewire storage
+    # Explanation : Best option is to use the install function, or else drivers can still be loaded manually
+    Register --test-no STRG-1846 --os Linux --weight L --network NO --category security --description "Check if firewire storage is disabled"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        FOUND=0
+        LogText "Test: Checking firewire storage driver in directory /etc/modprobe.d and configuration file /etc/modprobe.conf"
+        if [ -d ${ROOTDIR}etc/modprobe.d ]; then
+            FIND=$(${LSBINARY} ${ROOTDIR}etc/modprobe.d/* 2&gt; /dev/null)
+            if [ ! -z "${FIND}" ]; then
+                FIND1=$(${EGREPBINARY} "blacklist (ohci1394|firewire[-_]ohci|firewire-core)" ${ROOTDIR}etc/modprobe.d/* | ${GREPBINARY} -v "#")
+                FIND2=$(${EGREPBINARY} "install (ohci1394|firewire[-_]ohci|firewire-core) /bin/(false|true)" ${ROOTDIR}etc/modprobe.d/* | ${GREPBINARY} -v "#")
+                if [ ! -z "${FIND1}" -o ! -z "${FIND2}" ]; then
+                    FOUND=1
+                    LogText "Result: found firewire ohci driver in disabled state"
+                fi
+            else
+                LogText "Result: skipping ${ROOTDIR}etc/modprobe.d, directory found but no files in it"
+            fi
+        fi
+        if [ -f ${ROOTDIR}etc/modprobe.conf ]; then
+            FIND1=$(${EGREPBINARY} -r "blacklist (ohci1394|firewire[-_]ohci|firewire-core)" ${ROOTDIR}etc/modprobe.conf | ${GREPBINARY} -v "#")
+            FIND2=$(${EGREPBINARY} -r "install (ohci1394|firewire[-_]ohci|firewire-core) /bin/(false|true)" ${ROOTDIR}etc/modprobe.conf | ${GREPBINARY} -v "#")
+            if [ ! -z "${FIND1}" -o ! -z "${FIND2}" ]; then
+                FOUND=1
+                LogText "Result: found firewire ohci driver in disabled state"
+            fi
+        fi
+        if [ ${FOUND} -eq 0 ]; then
+            LogText "Result: firewire ohci driver is not explicitly disabled"
+            Display --indent 2 --text "- Checking firewire ohci driver (modprobe config)" --result "NOT DISABLED" --color WHITE
+            ReportSuggestion ${TEST_NO} "Disable drivers like firewire storage when not used, to prevent unauthorized storage or data theft"
+            # after blacklisting modules, make sure to remove them from the initram filesystem: update-initramfs -u
+            AddHP 2 3
+        else
+            LogText "Result: firewire ohci driver is disabled"
+            Display --indent 2 --text "- Checking firewire ohci driver (modprobe config)" --result "${STATUS_DISABLED}" --color GREEN
+            AddHP 3 3
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1902
+    # Description : Check rpcinfo
+    if [ ! -z "${RPCINFOBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no STRG-1902 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check rpcinfo registered programs"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking rpcinfo registered programs"
+        FIND=$(${RPCINFOBINARY} -p 2&gt; /dev/null | ${TRBINARY} -s ' ' ',')
+        for I in ${FIND}; do
+            LogText "rpcinfo: ${I}"
+        done
+        Display --indent 2 --text "- Query rpc registered programs" --result "${STATUS_DONE}" --color GREEN
+    fi</t>
+  </si>
+  <si>
+    <t>nfs versions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1904
+    # Description : Check nfs versions in rpcinfo
+    if [ ! -z "${RPCINFOBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no STRG-1904 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check nfs rpc"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking NFS registered versions"
+        FIND=$(${RPCINFOBINARY} -p 2&gt; /dev/null | ${AWKBINARY} '{ if ($5=="nfs") { print $2 } }' | uniq | sort)
+        for I in ${FIND}; do
+            LogText "Found version: ${I}"
+        done
+        Display --indent 2 --text "- Query NFS versions" --result "${STATUS_DONE}" --color GREEN
+    fi
+#</t>
+  </si>
+  <si>
+    <t>nfs protocols</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1906
+    # Description : Check nfs protocols (TCP/UDP) and port in rpcinfo
+    if [ ! -z "${RPCINFOBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no STRG-1906 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check nfs rpc"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking NFS registered protocols"
+        FIND=$(${RPCINFOBINARY} -p 2&gt; /dev/null | ${AWKBINARY} '{ if ($5=="nfs") { print $3 } }' | uniq | sort)
+        for I in ${FIND}; do
+            LogText "Found protocol: ${I}"
+        done
+        if [ -z "${FIND}" ]; then
+            LogText "Output: no NFS protocols found"
+        fi
+        # Check port number
+        LogText "Test: Checking NFS registered ports"
+        FIND=$(${RPCINFOBINARY} -p 2&gt; /dev/null | ${AWKBINARY} '{ if ($5=="nfs") { print $3 } }' | uniq | sort)
+        for I in ${FIND}; do
+            LogText "Found port: ${I}"
+        done
+        if [ -z "${FIND}" ]; then
+            LogText "Output: no NFS port number found"
+        fi
+        Display --indent 2 --text "- Query NFS protocols" --result "${STATUS_DONE}" --color GREEN
+    fi
+#</t>
+  </si>
+  <si>
+    <t>nfs daemons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1920
+    # Description : Check for running NFS daemons
+    Register --test-no STRG-1920 --weight L --network NO --category security --description "Checking NFS daemon"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking running NFS daemon"
+        FIND=$(${PSBINARY} ax | ${GREPBINARY} "nfsd" | ${GREPBINARY} -v "grep")
+        if [ -z "${FIND}" ]; then
+            LogText "Output: NFS daemon is not running"
+            Display --indent 2 --text "- Check running NFS daemon" --result "${STATUS_NOT_FOUND}" --color WHITE
+        else
+            LogText "Output: NFS daemon is running"
+            Display --indent 2 --text "- Check running NFS daemon" --result "${STATUS_FOUND}" --color GREEN
+            NFS_DAEMON_RUNNING=1
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>missing nfs in rpcinfo while nfs is running</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1924
+    # Description : Check missing nfs in rpcinfo while NFS is running
+    #Register --test-no STRG-1924 --weight L --network NO --category security --description "Checking NFS daemon"
+    #if [ ${SKIPTEST} -eq 0 ]; then
+#</t>
+  </si>
+  <si>
+    <t>nfs exports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1926
+    # Description : Check NFS exports
+    if [ ${NFS_DAEMON_RUNNING} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no STRG-1926 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Checking NFS exports"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: check /etc/exports"
+        if [ -f ${ROOTDIR}etc/exports ]; then
+            LogText "Result: ${ROOTDIR}etc/exports exists"
+            FIND=$(${GREPBINARY} -v "^$" ${ROOTDIR}etc/exports | ${GREPBINARY} -v "^#" | ${SEDBINARY} 's/ /!space!/g')
+            if [ ! -z "${FIND}" ]; then
+                for I in ${FIND}; do
+                    I=$(echo ${I} | ${SEDBINARY} 's/!space!/ /g')
+                    LogText "Found line: ${I}"
+                done
+            else
+                LogText "Result: ${ROOTDIR}etc/exports does not contain exported file systems"
+                NFS_EXPORTS_EMPTY=1
+            fi
+            Display --indent 4 --text "- Checking ${ROOTDIR}etc/exports" --result "${STATUS_FOUND}" --color GREEN
+        else
+            LogText "Result: file /etc/exports does not exist"
+            Display --indent 4 --text "- Checking ${ROOTDIR}etc/exports" --result "${STATUS_NOT_FOUND}" --color WHITE
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>empty exports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1928
+    # Description : Check for empty exports file while NFS is running
+    if [ ${NFS_DAEMON_RUNNING} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no STRG-1928 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Checking empty /etc/exports"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        if [ ${NFS_EXPORTS_EMPTY} -eq 1 ]; then
+            Display --indent 6 --text "- Checking empty /etc/exports" --result "${STATUS_SUGGESTION}" --color YELLOW
+            LogText "Result: ${ROOTDIR}etc/exports seems to have no exported file systems"
+            ReportSuggestion ${TEST_NO} "/etc/exports has no exported file systems, while NFS daemon is running. Check if NFS needs to run on this system"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>client access to NFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1930
+    # Description : Check client access to nfs share
+    if [ ${NFS_DAEMON_RUNNING} -eq 1 -a ${NFS_EXPORTS_EMPTY} -eq 0 -a ! "${SHOWMOUNTBINARY}" = "" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no STRG-1930 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check client access to nfs share"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        sFIND=$(${SHOWMOUNTBINARY} -e | ${AWKBINARY} '{ print $2 }' | ${SEDBINARY} '1d' | ${GREPBINARY} "\*")
+        if [ ! -z "${sFIND}" ]; then
+            LogText "Result: all client are allowed to access a NFS share in /etc/exports"
+            Display --indent 4 --text "- Checking NFS client access" --result "ALL CLIENTS" --color YELLOW
+            ReportSuggestion ${TEST_NO} "Specify clients that are allowed to access a NFS share /etc/exports"
+            AddHP 2 3
+        else
+            LogText "Result: only some clients are allowed to access a NFS share"
+            Display --indent 4 --text "- Checking NFS client access" --result "${STATUS_OK}" --color GREEN
+            AddHP 3 3
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>File integrity tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if [ -x ${ROOTDIR}/usr/bin/csrutil ]; then PREQS_MET="YES"; else PREQS_MET="NO"; SKIPREASON="No CSrutil binary found"; fi
+    Register --test-no SINT-7010 --preqs-met ${PREQS_MET} --skip-reason "${SKIPREASON}" --weight H --network NO --category security --description "System Integrity Status"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        if ${ROOTDIR}usr/bin/csrutil status | ${GREPBINARY} -sq enabled ; then
+            Display --indent 2 --text "- System Integrity Protectioni (status)" --result "${STATUS_OK}" --color GREEN
+            Report "system_integrity_tool[]=mac-sip"
+            LogText "Result: SIP enabled, OK"
+            AddHP 3 3
+        else
+            Display --indent 2 --text "- System Integrity Protection (status)" --result "${STATUS_NO}" --color RED
+            LogText "Result: SIP disabled, BAD"
+            AddHP 0 3
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>ntp daemon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3104
+    # Description : Check for a running NTP daemon
+    if [ -f /sys/hypervisor/type ]; then
+        # TODO: Skip NTP tests if we are in a DomU xen instance
+        FIND=$(cat /sys/hypervisor/type)
+        if [ "${FIND}" = "xen" ]; then PREQS_MET="NO"; else PREQS_MET="YES"; fi
+    elif [ -f /sbin/sysctl ] &amp;&amp; [ "$(/sbin/sysctl -n security.jail.jailed 2&gt;/dev/null || echo 0)" -eq 1 ]; then
+        # Skip NTP tests if we're in a FreeBSD jail
+        PREQS_MET="NO"
+    else
+        PREQS_MET="YES"
+    fi
+    Register --test-no TIME-3104 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check for running NTP daemon or client"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        # Linux/FreeBSD (ntpdate), OpenBSD (ntpd, rdate), Chrony, systemd-timesyncd
+        LogText "Test: Searching for a running NTP daemon or available client"
+        FOUND=0
+        SEARCH_FILES="${ROOTDIR}etc/chrony.conf ${ROOTDIR}etc/chrony/chrony.conf"
+        for FILE in ${SEARCH_FILES}; do
+            if [ -f ${FILE} ]; then LogText "result: found chrony configuration: ${FILE}"; CHRONY_CONF_FILE="${FILE}"; fi
+        done
+        if [ ! -z "${CHRONY_CONF_FILE}" ]; then
+            IsRunning chronyd
+            if [ ${RUNNING} -eq 1 ]; then
+                FOUND=1; NTP_DAEMON_RUNNING=1; NTP_CONFIG_TYPE_DAEMON=1; NTP_DAEMON="chronyd"
+                Display --indent 2 --text "- NTP daemon found: chronyd" --result "${STATUS_FOUND}" --color GREEN
+            else
+                LogText "Result: found chrony configuration, but no running daemon"
+            fi
+        else
+            LogText "Result: no chrony configuration found"
+        fi
+        # Check time daemon (eg DragonFly BSD)
+        IsRunning dntpd
+        if [ ${RUNNING} -eq 1 ]; then
+            FOUND=1; NTP_DAEMON_RUNNING=1; NTP_CONFIG_TYPE_DAEMON=1; NTP_DAEMON="dntpd"
+            Display --indent 2 --text "- NTP daemon found: dntpd" --result "${STATUS_FOUND}" --color GREEN
+        fi
+        # Check running processes
+        FIND=$(${PSBINARY} ax | ${GREPBINARY} "ntpd" | ${GREPBINARY} -v "dntpd" | ${GREPBINARY} -v "grep")
+        if [ ! -z "${FIND}" ]; then
+            FOUND=1; NTPD_RUNNING=1; NTP_DAEMON_RUNNING=1; NTP_CONFIG_TYPE_DAEMON=1
+            NTP_DAEMON="ntpd"
+            LogText "Result: found running NTP daemon in process list"
+            Display --indent 2 --text "- NTP daemon found: ntpd" --result "${STATUS_FOUND}" --color GREEN
+        fi
+        # Check time daemon (eg NetBSD)
+        IsRunning timed
+        if [ ${RUNNING} -eq 1 ]; then
+            FOUND=1; NTP_DAEMON_RUNNING=1; NTP_CONFIG_TYPE_DAEMON=1; NTP_DAEMON="timed"
+            Display --indent 2 --text "- NTP daemon found: timed" --result "${STATUS_FOUND}" --color GREEN
+        fi
+        # Check timedate daemon (systemd)
+        if [ ! -z "${TIMEDATECTL}" ]; then
+            FIND=$(${TIMEDATECTL} status | ${EGREPBINARY} "(NTP|System clock) synchronized: yes")
+            if [ ! -z "${FIND}" ]; then
+                # Check for systemd-timesyncd
+                if [ -f /etc/systemd/timesyncd.conf ]; then
+                    FOUND=1; NTP_DAEMON_RUNNING=1; NTP_CONFIG_TYPE_DAEMON=1; NTP_DAEMON="systemd-timesyncd"
+                    Display --indent 2 --text "- NTP daemon found: systemd (timesyncd)" --result "${STATUS_FOUND}" --color GREEN
+                    SYSTEMD_NTP_ENABLED=1
+                fi
+            else
+                LogText "Result: time sychronization not performed according timedatectl command"
+            fi
+        fi
+        # Check crontab for OpenBSD/FreeBSD
+        # Check anacrontab for Linux
+        CRONTAB_FILES="/etc/anacrontab /etc/crontab"
+        for I in ${CRONTAB_FILES}; do
+            if [ -f ${I} ]; then
+                LogText "Test: checking for ntpdate or rdate in crontab file ${I}"
+                FIND=$(${EGREPBINARY} "ntpdate|rdate" ${I} | ${GREPBINARY} -v '^#')
+                if [ ! -z "${FIND}" ]; then
+                    FOUND=1; NTP_CONFIG_TYPE_SCHEDULED=1
+                    Display --indent 2 --text "- Checking NTP client in crontab file (${I})" --result "${STATUS_FOUND}" --color GREEN
+                    LogText "Result: found ntpdate or rdate reference in crontab file ${I}"
+                else
+                    #Display --indent 2 --text "- Checking NTP client in crontab file (${I})" --result "${STATUS_NOT_FOUND}" --color WHITE
+                    LogText "Result: no ntpdate or rdate reference found in crontab file ${I}"
+                fi
+            else
+                LogText "Result: crontab file ${I} not found"
+            fi
+        done
+        # Don't run check in cron job directory on Solaris
+        # /etc/cron.d/FIFO is a special file and test get stuck at this file
+        FOUND_IN_CRON=0
+        # Check cron jobs
+        for I in ${CRON_DIRS}; do
+            if [ -d ${I} ]; then
+                if FileIsReadable ${I}; then
+                    FIND=$(${LSBINARY} ${I} | ${GREPBINARY} -v FIFO)
+                    if [ ! -z "${FIND}" ]; then
+                        for J in ${FIND}; do
+                            LogText "Test: checking for ntpdate or rdate in ${I}/${J}"
+                            FIND2=$(${EGREPBINARY} "rdate|ntpdate" ${I}/${J} | ${GREPBINARY} -v "^#")
+                            if [ ! -z "${FIND2}" ]; then
+                                LogText "Positive match found: ${FIND2}"
+                                FOUND=1; FOUND_IN_CRON=1; NTP_CONFIG_TYPE_SCHEDULED=1
+                            fi
+                        done
+                    else
+                        LogText "Result: ${I} is empty, skipping search in directory"
+                    fi
+                else
+                    LogText "Result: could not search in directory due to permissions"
+                fi
+            fi
+        done
+        if [ ${FOUND_IN_CRON} -eq 1 ]; then
+            Display --indent 2 --text "- Checking NTP client in cron files" --result "${STATUS_FOUND}" --color GREEN
+            LogText "Result: found ntpdate or rdate in cron directory"
+        else
+            LogText "Result: no ntpdate or rdate found in cron directories"
+        fi
+        # Checking if ntpdate is performed by event
+        LogText "Test: checking for file /etc/network/if-up.d/ntpdate"
+        if [ -f /etc/network/if-up.d/ntpdate ]; then
+            LogText "Result: found ntpdate action when network interface comes up"
+            FOUND=1
+            NTP_CONFIG_TYPE_EVENTBASED=1
+            Display --indent 2 --text "- Checking event based ntpdate (if-up)" --result "${STATUS_FOUND}" --color GREEN
+        else
+            LogText "Result: file /etc/network/if-up.d/ntpdate does not exist"
+        fi
+        # Configuration file for *BSD
+        if [ -f /etc/rc.conf ]; then
+            LogText "Test: Checking if ntpdate is enabled at startup in *BSD"
+            FIND=$(${GREPBINARY} 'ntpdate_enable="YES"' /etc/rc.conf)
+            if [ ! -z "${FIND}" ]; then
+                LogText "Result: ntpdate is enabled in rc.conf"
+                FOUND=1
+                NTP_CONFIG_TYPE_STARTUP=1
+                # Only show suggestion when ntpdate is enabled, however ntpd is not running
+                if [ ${NTP_DAEMON_RUNNING} -eq 0 ]; then
+                    ReportSuggestion ${TEST_NO} "Although ntpdate is enabled in rc.conf, it is advised to run it at least daily or use a NTP daemon"
+                fi
+            else
+                LogText "Result: ntpdate is not enabled in rc.conf"
+            fi
+        fi
+        if [ ${FOUND} -eq 0 ]; then
+            if [ ${ISVIRTUALMACHINE} -eq 1 ]; then
+                LogText "Result: Skipping display warning, as virtual machines usually don't need time synchronization in the VM itself"
+            else
+                Display --indent 2 --text "- Checking for a running NTP daemon or client" --result "${STATUS_WARNING}" --color RED
+                LogText "Result: Could not find a NTP daemon or client"
+                ReportSuggestion ${TEST_NO} "Use NTP daemon or NTP client to prevent time issues."
+                AddHP 0 2
+            fi
+        else
+            Display --indent 2 --text "- Checking for a running NTP daemon or client" --result "${STATUS_OK}" --color GREEN
+            LogText "Result: Found a time syncing daemon/client."
+            AddHP 3 3
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>systemd time sync</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3106
+    # Description : Check status of systemd time synchronization
+    if [ ${SYSTEMD_NTP_ENABLED} -eq 1 -a ! -z "${TIMEDATECTL}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no TIME-3106 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check systemd NTP time synchronization status"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Check the status of time synchronization via timedatectl"
+        FIND=$(${TIMEDATECTL} status | ${EGREPBINARY} "(NTP|System clock) synchronized: yes")
+        if [ -z "${FIND}" ]; then
+            LogText "Result: time not synchronized via NTP"
+            ReportSuggestion "${TEST_NO}" "Check timedatectl output. Sychronization via NTP is enabled, but status reflects it is not synchronized"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>associations from ntpq peers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3112
+    # Description : Check for valid associations from ntpq peers list
+    if [ ${NTPD_RUNNING} -eq 1 -a ! -z "${NTPQBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no TIME-3112 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check active NTP associations ID's"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking for NTP association ID's from ntpq peers list"
+        FIND=$(${NTPQBINARY} -p -n | ${GREPBINARY} "No association ID's returned")
+        if [ -z "${FIND}" ]; then
+            Display --indent 2 --text "- Checking valid association ID's" --result "${STATUS_FOUND}" --color GREEN
+            LogText "Result: Found one or more association ID's"
+        else
+            Display --indent 2 --text "- Checking valid association ID's" --result "${STATUS_WARNING}" --color RED
+            ReportSuggestion ${TEST_NO} "Check ntp.conf for properly configured NTP servers and a correctly functioning name service."
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>stratum 16 peers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3116
+    # Description : Check for stratum 16 peers
+    if [ ${NTPD_RUNNING} -eq 1 -a ! -z "${NTPQBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no TIME-3116 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check peers with stratum value of 16"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        COUNT=0
+        LogText "Test: Checking stratum 16 sources from ntpq peers list"
+        FIND=$(${NTPQBINARY} -p -n | ${AWKBINARY} '{ if ($2!=".POOL." &amp;&amp; $3=="16") { print $1 }}')
+        if [ -z "${FIND}" ]; then
+            Display --indent 2 --text "- Checking high stratum ntp peers" --result "${STATUS_OK}" --color GREEN
+            LogText "Result: All peers are lower than stratum 16"
+        else
+            for ITEM in ${FIND}; do
+                LogText "Found stratum 16 peer: ${ITEM}"
+                FIND2=$(${EGREPBINARY} "^ntp-ignore-stratum-16-peer=${ITEM}" ${PROFILE})
+                if IsEmpty "${FIND2}"; then
+                    COUNT=$((COUNT + 1))
+                    Report "ntp_stratum_16_peer[]=${ITEM}"
+                else
+                    LogText "Output: host ${ITEM} ignored by profile"
+                fi
+            done
+            # Check if one or more high stratum time servers are found
+            if [ ${COUNT} -eq 0 ]; then
+                Display --indent 2 --text "- Checking high stratum ntp peers" --result "${STATUS_OK}" --color GREEN
+                LogText "Result: all non local servers are lower than stratum 16, or whitelisted within the scan profile"
+            else
+                Display --indent 2 --text "- Checking high stratum ntp peers" --result "${STATUS_WARNING}" --color RED
+                LogText "Result: Found ${COUNT} high stratum (16) peers)"
+                ReportSuggestion ${TEST_NO} "Check ntpq peers output for stratum 16 peers"
+            fi
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>unreliable peers from peer list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3120
+    # Description : Check unreliable peers from peer list
+    # Notes       : Items with # are too far away (network distance)
+    #               Items with - are not chosen due clustering algorithm
+    if [ ${NTPD_RUNNING} -eq 1 -a ! -z "${NTPQBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no TIME-3120 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check unreliable NTP peers"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking unreliable ntp peers"
+        FIND=$(${NTPQBINARY} -p -n | ${EGREPBINARY} "^(-|#)" | ${AWKBINARY} '{ print $1 }' | ${SEDBINARY} 's/^-//g')
+        if [ -z "${FIND}" ]; then
+            Display --indent 2 --text "- Checking unreliable ntp peers" --result "${STATUS_NONE}" --color GREEN
+            LogText "Result: No unreliable peers found"
+        else
+            Display --indent 2 --text "- Checking unreliable ntp peers" --result "${STATUS_FOUND}" --color YELLOW
+            LogText "Result: Found one or more unreliable peers (marked with a minus or dash sign)"
+            for I in ${FIND}; do
+                LogText "Unreliable peer: ${I}"
+                Report "ntp_unreliable_peer[]=${I}"
+            done
+            ReportSuggestion ${TEST_NO} "Check ntpq peers output for unreliable ntp peers and correct/replace them"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>check selected time source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3124
+    # Description : Check selected time source
+    if [ ${NTPD_RUNNING} -eq 1 -a ! -z "${NTPQBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no TIME-3124 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check selected time source"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking selected time source"
+        FIND=$(${NTPQBINARY} -p -n | ${GREPBINARY} '^*' | ${AWKBINARY} '{ if ($4=="l") { print $1 } }')
+        FIND2=$(${NTPQBINARY} -p -n | ${GREPBINARY} '^*' | ${AWKBINARY} '{ print $1 }')
+        if [ -z "${FIND}" -a ! -z "${FIND2}" ]; then
+            Display --indent 2 --text "- Checking selected time source" --result "${STATUS_OK}" --color GREEN
+            FIND2=$(echo ${FIND2} | ${SEDBINARY} 's/*//g')
+            LogText "Result: Found selected time source (value: ${FIND2})"
+        else
+            Display --indent 2 --text "- Checking selected time source" --result "${STATUS_WARNING}" --color RED
+            LogText "Result: Found local source as selected time source. This could indicate that no external sources are available to sync with."
+            LogText "Local source: ${FIND}"
+            ReportSuggestion ${TEST_NO} "Check ntpq peers output for selected time source"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>check time source candidates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3128
+    # Description : Check time source candidates
+    if [ ${NTPD_RUNNING} -eq 1 -a ! -z "${NTPQBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no TIME-3128 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check preferred time source"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking preferred time source"
+        FIND=$(${NTPQBINARY} -p -n | ${GREPBINARY} '^+' | ${AWKBINARY} '{ print $1 }')
+        if [ -z "${FIND}" ]; then
+            Display --indent 2 --text "- Checking time source candidates" --result "${STATUS_NONE}" --color YELLOW
+            LogText "Result: No other time source candidates found"
+            ReportSuggestion ${TEST_NO} "Check ntpq peers output for time source candidates"
+        else
+            Display --indent 2 --text "- Checking time source candidates" --result "${STATUS_OK}" --color GREEN
+            LogText "Result: Found one or more candidates to synchronize time with."
+            for I in ${FIND}; do
+                I=$(echo ${I} | ${SEDBINARY} 's/+//g')
+                LogText "Candidate found: ${I}"
+            done
+        fi
+    fi</t>
+  </si>
+  <si>
+    <t>ntp falsetickers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3132
+    # Description : Check ntpq falsetickers
+    if [ ${NTPD_RUNNING} -eq 1 -a ! -z "${NTPQBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no TIME-3132 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check NTP falsetickers"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking preferred time source"
+        FIND=$(${NTPQBINARY} -p -n | ${EGREPBINARY} '^x')
+        if [ -z "${FIND}" ]; then
+            Display --indent 2 --text "- Checking falsetickers" --result "${STATUS_OK}" --color GREEN
+            LogText "Result: No falsetickers found (items preceeding with an 'x')"
+        else
+            Display --indent 2 --text "- Checking falsetickers" --result "${STATUS_NONE}" --color YELLOW
+            LogText "Result: Found one or more falsetickers  (items preceeding with an 'x')"
+            for I in ${FIND}; do
+                I=$(echo ${I} | ${SEDBINARY} 's/x//g')
+                LogText "Falseticker found: ${I}"
+                Report "ntp_falseticker[]=${I}"
+            done
+            ReportSuggestion ${TEST_NO} "Check ntpq peers output for falsetickers"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>ntpd version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3136
+    # Description : Check ntpq reported ntp version (Linux)
+    if [ ${NTPD_RUNNING} -eq 1 -a ! -z "${NTPQBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no TIME-3136 --os Linux --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check NTP protocol version"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking NTP protocol version (ntpq -c ntpversion)"
+        FIND=$(${NTPQBINARY} -c ntpversion | ${AWKBINARY} '{ if ($1=="NTP" &amp;&amp; $2=="version" &amp;&amp; $5=="is") { print $6 } }')
+        if [ -z "${FIND}" ]; then
+            Display --indent 2 --text "- Checking NTP version" --result "${STATUS_UNKNOWN}" --color YELLOW
+            LogText "Result: No NTP version found"
+            ReportSuggestion ${TEST_NO} "Check ntpq output for NTP protocol version"
+        else
+            Display --indent 2 --text "- Checking NTP version" --result "${STATUS_FOUND}" --color GREEN
+            LogText "Result: Found NTP version ${FIND}"
+            Report "ntp_version=${FIND}"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> /etc/default/ntpdate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3146
+    # Description : Check /etc/default/ntpdate (Linux)
+    # Notes       : ntpdate-debian binary
+    #if [ ${NTPD_RUNNING} -eq 1 -a ! -z "${NTPQBINARY}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    #Register --test-no TIME-3146 --os Linux --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check /etc/default/ntpdate"
+    #if [ ${SKIPTEST} -eq 0 ]; then
+#</t>
+  </si>
+  <si>
+    <t>TZ variable is set</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3148
+    # Description : Check if TZ variable is set (Linux)
+    # Notes       : without TZ variable set, a lot of unneeded calls might be performed.
+    Register --test-no TIME-3148 --os Linux --weight L --network NO --category performance --description "Check TZ variable"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: testing for TZ variable"
+        FIND="${TZ:=notset}"
+        LogText "Result: found TZ variable with value ${FIND}"
+        if [ "${FIND}" = "notset" ]; then
+            Report "tz_variable_empty=1"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>empty step-tickers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3160
+    # Description : Check empty NTP step-tickers
+    # Notes       : Mostly applies to Red Hat and clones
+    FILE="${ROOTDIR}etc/ntp/step-tickers"
+    if [ "${NTPD_RUNNING}" -eq 1 -a ! -z "${NTPQBINARY}" -a -f "${FILE}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no TIME-3160 --os Linux --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check empty NTP step-tickers"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        FOUND=0
+        OUTPUT=$(${AWKBINARY} '/^[a-z0-9]/ { print $1 }' ${FILE})
+        if [ -z "${OUTPUT}" ]; then
+            LogText "Result: ${FILE} is empty. The step-tickers contain no configured NTP servers"
+            Display --indent 2 --text "- Checking NTP step-tickers file" --result "EMPTY FILE" --color YELLOW
+            ReportSuggestion ${TEST_NO} "Use step-tickers file for quicker time synchronization"
+        else
+            LogText "Result: ${FILE} is not empty, which is fine"
+            Display --indent 2 --text "- Checking NTP step-tickers file" --result "${STATUS_OK}" --color GREEN
+            sFIND=$(${AWKBINARY} '/^[a-z0-9]/ { print $1 }' ${FILE} | ${EGREPBINARY} -v "^127." | ${EGREPBINARY} -v "^::1")
+            for I in ${sFIND}; do
+                FIND=$(${GREPBINARY} ^${I} ${FILE} | wc -l)
+                if [ ${FIND} -gt 0 ]; then
+                    LogText "Result: $I exist in ${FILE}"
+                else
+                    LogText "Result: ${I} does NOT exist in ${FILE}"
+                    FOUND=1
+                fi
+            done
+            if [ ${FOUND} -eq 1 ]; then
+                Display --indent 4 --text "- Checking step-tickers ntp servers entries" --result "SOME MISSING" --color YELLOW
+                ReportSuggestion ${TEST_NO} "Some time servers missing in step-tickers file"
+                AddHP 3 4
+            else
+                Display --indent 4 --text "- Checking step-tickers ntp servers entries" --result "${STATUS_OK}" --color GREEN
+                LogText "Result: all time servers are in step-tickers file"
+                AddHP 4 4
+            fi
+        fi
+        LogText "Information: step-tickers is used by ntpdate where as ntp.conf is the configuration file for the ntpd daemon. ntpdate is initially run to set the clock before ntpd to make sure time is within 1000 sec."
+        LogText "Risk: ntp will not run at boot if the time difference between the server and client by more then 1000 sec."
+    fi
+#</t>
+  </si>
+  <si>
+    <t>file permissions and ownership of configuration files</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TIME-3170
+    # Description : Check file permissions and ownership of configuration files
+    # Notes       : Files should be owned by root, or the user running
+    #               Group owner should have only read access
+    #               Other should preferably have no access, or read-only at max
+    FILE_ARRAY="${ROOTDIR}etc/chrony.conf ${ROOTDIR}usr/pkg/etc/chrony.conf \
+        ${ROOTDIR}etc/inet/ntp.conf ${ROOTDIR}etc/ntp.conf ${ROOTDIR}usr/local/etc/ntp.conf"
+    Register --test-no TIME-3170 --weight L --network NO --category security --description "Check configuration files"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        for FILE in ${FILE_ARRAY}; do
+            if [ -f ${FILE} ]; then
+                LogText "Result: found ${FILE}"
+                if IsWorldWritable ${FILE}; then
+                    ReportWarning "${TEST_NO}" "Found world writable configuration file" "${FILE}" ""
+                fi
+                Report "ntp_config_file[]=${FILE}"
+            fi
+        done
+    fi
+#</t>
+  </si>
+  <si>
+    <t>check for automation tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TOOL-5002
+    # Description : Check if automation tools are found
+    Register --test-no TOOL-5002 --weight L --network NO --category security --description "Checking for automation tools"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        Display --indent 2 --text "- Checking automation tooling"
+        # Ansible
+        FOUND=0
+        LIST="~/.ansible ${ROOTDIR}etc/ansible ${ROOTDIR}root/.ansible ${ROOTDIR}tmp/.ansible"
+        for ITEM in ${LIST}; do if DirectoryExists ${ITEM}; then FOUND=1; break; fi; done
+        # Test for files (only if no match was found)
+        if [ ${FOUND} -eq 0 ]; then
+            LIST="${ROOTDIR}var/log/ansible.log ~/.ansible-retry"
+            for ITEM in ${LIST}; do if FileExists ${ITEM}; then FOUND=1; break; fi; done
+        fi
+        if [ ${FOUND} -eq 1 ]; then
+            LogText "Result: found a possible trace of Ansible"
+            AUTOMATION_TOOL_FOUND=1
+            ANSIBLE_ARTIFACT_FOUND=1
+            Report "automation_tool_running[]=ansible"
+            Display --indent 4 --text "- Ansible artifact" --result "${STATUS_FOUND}" --color GREEN
+        fi
+        # Cfengine
+        if [ ! -z "${CFAGENTBINARY}" ]; then
+            LogText "Result: CFEngine (cfagent) is installed (${CFAGENTBINARY})"
+            AUTOMATION_TOOL_FOUND=1
+            CFENGINE_AGENT_FOUND=1
+            Report "automation_tool_running[]=cf-agent"
+            Display --indent 4 --text "- Cfengine (cfagent)" --result "${STATUS_FOUND}" --color GREEN
+        fi
+        OTHER_CFENGINE_LOCATIONS="/var/cfengine/bin /var/rudder/cfengine-community/bin"
+        for I in ${OTHER_CFENGINE_LOCATIONS}; do
+            if [ -d ${I} ]; then
+                if [ -f ${I}/cf-agent ]; then
+                    LogText "Result: found CFEngine agent (cf-agent) in ${I}"
+                    AUTOMATION_TOOL_FOUND=1
+                    CFENGINE_AGENT_FOUND=1
+                    Report "automation_tool_running[]=cf-agent"
+                    Display --indent 4 --text "- CFEngine (cf-agent)" --result "${STATUS_FOUND}" --color GREEN
+                fi
+                if IsRunning "cf-server"; then
+                    LogText "Result: found CFEngine server"
+                    AUTOMATION_TOOL_FOUND=1
+                    CFENGINE_SERVER_RUNNING=1
+                    Report "automation_tool_running[]=cf-server"
+                    Display --indent 4 --text "- CFEngine (cf-server)" --result "${STATUS_FOUND}" --color GREEN
+                fi
+            fi
+        done
+        # Chef
+        CHEF_LOCATIONS="/opt/chef/bin /opt/chef-server/sv /opt/chefdk/bin"
+        for I in ${CHEF_LOCATIONS}; do
+            if [ -d ${I} ]; then
+                if [ -f ${I}/chef-client ]; then
+                    CHEFCLIENTBINARY="${I}/chef-client"
+                    AUTOMATION_TOOL_FOUND=1
+                    Report "automation_tool_running[]=chef-client"
+                    Display --indent 4 --text "- Chef client (chef-client)" --result "${STATUS_FOUND}" --color GREEN
+                    LogText "Result: found chef-client (chef client daemon) in ${I}"
+                fi
+                if [ -f ${I}/erchef ]; then
+                    CHEFSERVERBINARY="${I}/erchef"
+                    LogText "Result: Chef Server (erchef) is installed (${CHEFSERVERBINARY})"
+                    AUTOMATION_TOOL_FOUND=1
+                    Report "automation_tool_running[]=chef-server"
+                    Display --indent 4 --text "- Chef Server (erchef)" --result "${STATUS_FOUND}" --color GREEN
+                    LogText "Result: found erchef (chef server daemon) in ${I}"
+                fi
+            fi
+        done
+        # Puppet
+        # Check for Puppet installation provided by Puppetlabs package
+        if [ -z "${PUPPETBINARY}" ]; then
+            if [ -f ${ROOTDIR}opt/puppetlabs/puppet/bin/puppet ]; then
+                PUPPETBINARY="${ROOTDIR}opt/puppetlabs/puppet/bin/puppet"
+            fi
+        fi
+        if [ ! -z "${PUPPETBINARY}" ]; then
+            LogText "Result: Puppet is installed (${PUPPETBINARY})"
+            AUTOMATION_TOOL_FOUND=1
+            Report "automation_tool_running[]=puppet-agent"
+            Display --indent 4 --text "- Puppet (agent)" --result "${STATUS_FOUND}" --color GREEN
+        fi
+        if IsRunning --full "puppet master"; then
+            LogText "Result: found puppet master"
+            AUTOMATION_TOOL_FOUND=1
+            PUPPET_MASTER_RUNNING=1
+            Report "automation_tool_running[]=puppet-master"
+            Display --indent 4 --text "- Puppet (master)" --result "${STATUS_FOUND}" --color GREEN
+        fi
+        # SaltStack
+        if [ ! -z "${SALTMINIONBINARY}" ]; then
+            LogText "Result: SaltStack (salt-minion) is installed (${SALTMINIONBINARY})"
+            AUTOMATION_TOOL_FOUND=1
+            SALT_MINION_RUNNING=1
+            Report "automation_tool_running[]=saltstack-minion"
+            Display --indent 4 --text "- SaltStack minion (salt-minion)" --result "${STATUS_FOUND}" --color GREEN
+        fi
+        if [ ! -z "${SALTMASTERBINARY}" ]; then
+            LogText "Result: SaltStack (salt-master) is installed (${SALTMASTERBINARY})"
+            AUTOMATION_TOOL_FOUND=1
+            SALT_MASTER_RUNNING=1
+            Report "automation_tool_running[]=saltstack-minion"
+            Display --indent 4 --text "- SaltStack master (salt-master)" --result "${STATUS_FOUND}" --color GREEN
+        else
+            if IsRunning "salt-master"; then
+                LogText "Result: found SaltStack (master)"
+                AUTOMATION_TOOL_FOUND=1
+                SALT_MASTER_RUNNING=1
+                Report "automation_tool_running[]=saltstack-master"
+                Display --indent 4 --text "- SaltStack (master)" --result "${STATUS_FOUND}" --color GREEN
+            fi
+        fi
+        if [ ${AUTOMATION_TOOL_FOUND} -eq 1 ]; then
+            Display --indent 2 --text "- Automation tooling" --result "${STATUS_FOUND}" --color GREEN
+        else
+            Display --indent 2 --text "- Automation tooling" --result "${STATUS_NOT_FOUND}" --color YELLOW
+            ReportSuggestion ${TEST_NO} "Determine if automation tools are present for system management"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ansible
+cfengine
+chef
+puppet
+saltstack
+</t>
+  </si>
+  <si>
+    <t>fail2ban</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TOOL-5102
+    # Description : Check for Fail2ban
+    Register --test-no TOOL-5102 --weight L --network NO --category security --description "Check for presence of Fail2ban"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        # Fail2ban presence
+        if [ ! -z "${FAIL2BANBINARY}" ]; then
+            FAIL2BAN_FOUND=1
+            IDS_IPS_TOOL_FOUND=1
+            LogText "Result: Fail2ban is installed (${FAIL2BANBINARY})"
+            Report "ids_ips_tooling[]=fail2ban"
+            Display --indent 2 --text "- Checking presence of Fail2ban" --result "${STATUS_FOUND}" --color GREEN
+        else
+            LogText "Result: Fail2ban not present (fail2ban-server not found)"
+        fi
+        # Fail2ban configuration
+        LogText "Checking Fail2ban configuration file"
+        if [ -f /etc/fail2ban/jail.local ]; then
+            FAIL2BAN_CONFIG="/etc/fail2ban/jail.local"
+        elif [ -f /etc/fail2ban/jail.conf ]; then
+            FAIL2BAN_CONFIG="/etc/fail2ban/jail.conf"
+        else
+            FAIL2BAN_CONFIG=""
+        fi
+        # Continue if tooling is available and configuration file found
+        if [ ${FAIL2BAN_FOUND} -eq 1 -a ! -z "${FAIL2BAN_CONFIG}" ]; then
+            Report "fail2ban_config=${FAIL2BAN_CONFIG}"
+            FAIL2BANCLIENT=$(which fail2ban-client 2&gt; /dev/null | grep -v "no [^ ]* in ")
+            if [ ! -z "${FAIL2BANCLIENT}" ]; then PERFORM_FAIL2BAN_TESTS=1; fi
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>fail2ban enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TOOL-5104
+    # Description : Check for Fail2ban enabled tests
+    if [ ${PERFORM_FAIL2BAN_TESTS} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no TOOL-5104 --weight L --network NO --preqs-met ${PREQS_MET} --category security --description "Enabled tests in Fail2ban"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        FIND=$(${FAIL2BANCLIENT} -d | ${TRBINARY} -d '[]' | ${TRBINARY} -d "'" | ${AWKBINARY} -F, '{ if ($1=="add") { print $2 }}' | ${TRBINARY} -d ' ')
+        if [ ! -z "${FIND}" ]; then
+            for F2BSERVICE in ${FIND}; do
+                LogText "Result: service '${F2BSERVICE}' enabled"
+                Report "fail2ban_enabled_service[]=${F2BSERVICE}"
+            done
+            LogText "Result: found at least one enabled jail"
+            Display --indent 4 --text "- Checking Fail2ban jails" --result "${STATUS_ENABLED}" --color GREEN
+            AddHP 3 3
+        else
+            LogText "Result: Fail2ban installed but completely disabled"
+            Display --indent 4 --text "- Checking Fail2ban jails" --result "${STATUS_DISABLED}" --color RED
+            AddHP 0 5
+            ReportWarning "${TEST_NO}" "All jails in Fail2ban are disabled" "${FAIL2BAN_CONFIG}"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>fail2ban configs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # These tests are temporarily disabled to split them up in different areas to check
+    #
+    #            LogText "Result: found configuration file (${FAIL2BAN_CONFIG})"
+    #
+    #            # Check email alert configuration
+    #            LogText "Test: checking for email actions within ${FAIL2BAN_CONFIG}"
+    #
+    #            FIND=$(${EGREPBINARY} "^action = \%\(action_m.*\)s" ${FAIL2BAN_CONFIG})
+    #            FIND2=$(${EGREPBINARY} "^action = \%\(action_\)s" ${FAIL2BAN_CONFIG})
+    #
+    #            if [ ! -z "${FIND}" ]; then
+    #                FAIL2BAN_EMAIL=1
+    #                LogText "Result: found at least one jail which sends an email alert"
+    #            fi
+    #
+    #            if [ ! -z "${FIND2}" ]; then
+    #                FAIL2BAN_SILENT=1
+    #                LogText "Result: found at least one jail which does NOT send an email alert"
+    #            fi
+    #
+    #            if [ ${FAIL2BAN_SILENT} -eq 0 ] &amp;&amp; [ ${FAIL2BAN_EMAIL} -eq 0 ]; then
+    #                LogText "No registered actions found in ${FAIL2BAN_CONFIG}"
+    #                Display --indent 4 --text "- Checking Fail2ban actions" --result "${STATUS_NONE}" --color RED
+    #                ReportWarning "${TEST_NO}" "${FAIL2BAN_CONFIG}" "There are no actions configured for Fail2ban."
+    #                AddHP 0 3
+    #            fi
+    #
+    #            if [ ${FAIL2BAN_SILENT} -eq 0 ] &amp;&amp; [ ${FAIL2BAN_EMAIL} -eq 1 ]; then
+    #                LogText "All actions in ${FAIL2BAN_CONFIG} are configured to send email alerts"
+    #                Display --indent 4 --text "- Checking Fail2ban actions" --result "${STATUS_OK}" --color GREEN
+    #                AddHP 3 3
+    #            fi
+    #
+    #            if [ ${FAIL2BAN_SILENT} -eq 1 ] &amp;&amp; [ ${FAIL2BAN_EMAIL} -eq 1 ]; then
+    #                LogText "Some actions found in ${FAIL2BAN_CONFIG} are configured to send email alerts"
+    #                Display --indent 4 --text "- Checking Fail2ban actions" --result PARTIAL --color YELLOW
+    #                ReportSuggestion "${TEST_NO}" "Some Fail2ban jails are configured with non-notified actions.  Consider changing these to emailed alerts."
+    #                AddHP 2 3
+    #            fi
+    #
+    #            if [ ${FAIL2BAN_SILENT} -eq 1 ] &amp;&amp; [ ${FAIL2BAN_EMAIL} -eq 0 ]; then
+    #                LogText "None of the actions found in ${FAIL2BAN_CONFIG} are configured to send email alerts"
+    #                Display --indent 4 --text "- Checking Fail2ban actions" --result "${STATUS_NONE}" --color YELLOW
+    #                ReportSuggestion "${TEST_NO}" "None of the Fail2ban jails are configured to send email notifications.  Consider changing these to emailed alerts."
+    #                AddHP 1 3
+    #            fi
+    #
+    #            # Check at least one enabled jail
+    #            LogText "Checking for enabled jails within ${FAIL2BAN_CONFIG}"
+    #
+    #
+    #
+    #            # Confirm at least one iptables chain for fail2ban
+    #
+    #            LogText "Checking for fail2ban iptables chains"
+    #
+    #            if [ ! -z "${IPTABLESBINARY}" ]; then
+    #                CHECK_CHAINS=$(${IPTABLESBINARY} -L 2&gt;&amp;1 | ${GREPBINARY} fail2ban)
+    #                if [ ! -z "${CHECK_CHAINS}" ]; then
+    #                    LogText "Result: found at least one iptables chain for fail2ban"
+    #                    Display --indent 4 --text "- Checking for Fail2ban iptables chain" --result "${STATUS_OK}" --color GREEN
+    #                else
+    #                    LogText "Result: Fail2ban installed but iptables chain not present - fail2ban will not work"
+    #                    Display --indent 4 --text "- Checking for Fail2ban iptables chain" --result "${STATUS_WARNING}" --color RED
+    #                    AddHP 0 3
+    #                    ReportSuggestion "${TEST_NO}" "Check config to see why iptables does not have a fail2ban chain" "${FAIL2BAN_CONFIG}"
+    #                fi
+    #            else
+    #                Display --indent 4 --text "- Checking for Fail2ban iptables chain" --result "${STATUS_WARNING}" --color RED
+    #                ReportSuggestion "${TEST_NO}" "iptables doesn't seem to be installed; Fail2ban will not work. Remove Fail2ban or install iptables" "${FAIL2BAN_CONFIG}"
+    #            fi
+    #        fi
+    #    fi
+#</t>
+  </si>
+  <si>
+    <t>check for snort</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TOOL-5120
+    # Description : Check for Snort
+    Register --test-no TOOL-5120 --weight L --network NO --category security --description "Check for presence of Snort"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        # Snort presence
+        if [ -n "${SNORTBINARY}" ]; then
+            SNORT_FOUND=1
+            IDS_IPS_TOOL_FOUND=1
+            LogText "Result: Snort is installed (${SNORTBINARY})"
+            Report "ids_ips_tooling[]=snort"
+            Display --indent 2 --text "- Checking presence of Snort" --result "${STATUS_FOUND}" --color GREEN
+        fi
+        if IsRunning "snort"; then
+            SNORT_FOUND=1
+            SNORT_RUNNING=1
+            SNORT_LOG=$(${PSBINARY} | ${AWKBINARY} -F-.. '/snort/ {print $4}' | ${HEADBINARY} -1)
+        else
+            LogText "Result: Snort not present (Snort not running)"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>check snort config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TOOL-5122
+    # Description : Check for Snort configuration
+    Register --test-no TOOL-5122 --weight L --network NO --category security --description "Check Snort configuration file"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        # Continue if tooling is available and snort is running
+        if [ -n ${SNORT_FOUND} ] || [ -n ${SNORT_RUNNING} ]; then
+            if [ ${SNORT_FOUND} -eq 1 ] &amp;&amp; [ ${SNORT_RUNNING} -eq 1 ]; then
+                SNORT_CONFIG=$(${PSBINARY} | ${AWKBINARY} -F-.. '/snort/ {print $3}' | ${HEADBINARY} -1)
+                if HasData "${SNORT_CONFIG}"; then
+                    LogText "Result: found Snort configuration file: ${SNORT_CONFIG}"
+                    Report "snort_config=${SNORT_CONFIG}"
+                fi
+                SNORT=$(which snort 2&gt; /dev/null)
+            fi
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>IDS/IPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : TOOL-5190
+    # Description : Check for an IDS/IPS tool
+    Register --test-no TOOL-5190 --weight L --network NO --category security --description "Check presence of IDS/IPS tool"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        if [ ${IDS_IPS_TOOL_FOUND} -eq 1 ]; then
+            Display --indent 2 --text "- Checking for IDS/IPS tooling" --result "${STATUS_FOUND}" --color GREEN
+            AddHP 2 2
+        else
+            Display --indent 2 --text "- Checking for IDS/IPS tooling" --result "${STATUS_NONE}" --color YELLOW
+            #ReportSuggestion ${TEST_NO} "Install and configure automated intrusion detection/prevention tools"
+            AddHP 0 2
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>disabled USB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1840 (future ID: USB-1200)
+    # Description : Check for disabled USB storage
+    Register --test-no STRG-1840 --os Linux --weight L --network NO --category security --description "Check if USB storage is disabled"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        FOUND=0
+        LogText "Test: Checking USB storage driver in directory /etc/modprobe.d and configuration file /etc/modprobe.conf"
+        if [ -d /etc/modprobe.d ]; then
+            FIND=$(${LSBINARY} ${ROOTDIR}etc/modprobe.d/* 2&gt; /dev/null)
+            if [ ! -z "${FIND}" ]; then
+                FIND=$(${EGREPBINARY} -r "install usb[-_]storage /bin/(false|true)" ${ROOTDIR}etc/modprobe.d/* | ${GREPBINARY} -v "#")
+                FIND2=$(${EGREPBINARY} -r "^blacklist usb[-_]storage" ${ROOTDIR}etc/modprobe.d/*)
+                if [ ! -z "${FIND}" -o ! -z "${FIND2}" ]; then
+                    FOUND=1
+                    LogText "Result: found usb-storage driver in disabled state (blacklisted)"
+                fi
+            else
+                LogText "Result: uncommon situation. Found /etc/modprobe.d directory, but no files in it."
+            fi
+        fi
+        if [ -f ${ROOTDIR}etc/modprobe.conf ]; then
+            FIND=$(${EGREPBINARY} "install usb[-_]storage /bin/(false|true)" ${ROOTDIR}etc/modprobe.conf | ${GREPBINARY} "usb-storage" | ${GREPBINARY} -v "#")
+            if [ ! -z "${FIND}" ]; then
+                FOUND=1
+                LogText "Result: found usb-storage driver in disabled state"
+            fi
+        fi
+        if [ ${FOUND} -eq 0 ]; then
+            LogText "Result: usb-storage driver is not explicitly disabled"
+            Display --indent 2 --text "- Checking usb-storage driver (modprobe config)" --result "NOT DISABLED" --color WHITE
+            if [ "${USBGUARD_FOUND}" -eq "0" ]; then
+                ReportSuggestion ${TEST_NO} "Disable drivers like USB storage when not used, to prevent unauthorized storage or data theft"
+            fi
+            AddHP 2 3
+        else
+            LogText "Result: usb-storage driver is disabled"
+            Display --indent 2 --text "- Checking usb-storage driver (modprobe config)" --result "${STATUS_DISABLED}" --color GREEN
+            AddHP 3 3
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>USB authorizations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : STRG-1842 (future ID: USB-2000)
+    # Description : Check USB authorizations
+    Register --test-no STRG-1842 --os Linux --weight L --network NO --category security --description "Check USB authorizations"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking USB devices authorization to connect to the system"
+        FOUND=0
+        USBDEVICESPATH="/sys/bus/usb/devices/usb"
+        for device in "${USBDEVICESPATH}"*; do
+            if [ -e "${device}/authorized" ] || [ -e "${device}/authorized_default" ]; then
+                if [ $(cat "${device}/authorized_default") -eq 1 ]; then
+                    FOUND=1
+                    LogText "Test: ${device} is authorized by default"
+                    Report "usb_authorized_default_device[]=${device}"
+                elif [ $(cat "${device}/authorized") -eq 1 ]; then
+                    FOUND=1
+                    LogText "Test: ${device} is authorized currently"
+                    Report "usb_authorized_device[]=${device}"
+                fi
+            fi
+        done
+        if [ ${FOUND} -eq 1 ]; then
+            LogText "Result: Some USB devices are authorized by default (or temporary) to connect to the system"
+            Display --indent 2 --text "- Checking USB devices authorization" --result "${STATUS_ENABLED}" --color YELLOW
+            # To-Be-Added: create documentation and enable the suggestion
+            #if [ ${USBGUARD_FOUND} -eq 0 ]; then
+            #   ReportSuggestion ${TEST_NO} "Disable USB devices authorization, to prevent unauthorized storage or data theft"
+            #fi
+            AddHP 0 3
+        else
+            LogText "Result: None USB devices are authorized by default (or temporary) to connect to the system"
+            Display --indent 2 --text "- Checking USB devices authorization" --result "${STATUS_DISABLED}" --color GREEN
+            AddHP 3 3
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>USBGuard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : USB-3000
+    # Description : Perform USBGuard check
+    Register --test-no USB-3000  --os Linux --weight L --network NO --category security --description "Check for presence of USBGuard"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        if [ ${USBGUARD_FOUND} -eq 1 ]; then
+            LogText "Result: USBGuard is installed (${USBGUARDBINARY})"
+            Display --indent 2 --text "- Checking USBGuard" --result "${STATUS_FOUND}" --color GREEN
+            AddHP 1 1
+            LogText "Checking USBGuard configuration file"
+            if [ -f /etc/usbguard/usbguard-daemon.conf ]; then
+                USBGUARD_CONFIG="/etc/usbguard/usbguard-daemon.conf"
+            else
+                USBGUARD_CONFIG=""
+            fi
+            if [ ! -z "${USBGUARD_CONFIG}" ]; then
+                LogText "Result: USBGuard configuration found (${USBGUARD_CONFIG})"
+                Display --indent 4 --text "- Configuration" --result "${STATUS_FOUND}" --color GREEN
+                AddHP 1 1
+                LogText "Checking USBGuard restore controller device state (RestoreControllerDeviceState)"
+                USBGUARD_RESTORE_POLICY=$(${AWKBINARY} -F '=' -v OPT="RestoreControllerDeviceState" 'index($0, OPT) == 1 {print $2}' ${USBGUARD_CONFIG})
+                if [ ! -z "${USBGUARD_RESTORE_POLICY}" ]; then
+                    LogText "Result: RestoreControllerDeviceState = ${USBGUARD_RESTORE_POLICY}"
+                    case "${USBGUARD_RESTORE_POLICY}" in
+                        "true")
+                            Display --indent 6 --text "- Restore controller device state" --result "${USBGUARD_RESTORE_POLICY}" --color YELLOW
+                            LogText "  Consider changing RestoreControllerDeviceState to \"false\""
+                            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                            # ReportSuggestion ${TEST_NO} "Consider hardening USBGuard configuration" "RestoreControllerDeviceState (${USBGUARD_RESTORE_POLICY} --&gt; false)"
+                            AddHP 0 1
+                            ;;
+                        "false")
+                            Display --indent 6 --text "- Restore controller device state" --result "${USBGUARD_RESTORE_POLICY}" --color GREEN
+                            AddHP 1 1
+                            ;;
+                        *)
+                            LogText "Result: Invalid configuration for RestoreControllerDeviceState"
+                            Display --indent 6 --text "- Restore controller device state" --result "Invalid" --color RED
+                            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                            # ReportSuggestion ${TEST_NO} "Fix USBGuard configuration" "RestoreControllerDeviceState invalid \"${USBGUARD_RESTORE_POLICY}\""
+                            AddHP 0 1
+                            ;;
+                    esac
+                else
+                    LogText "Result: RestoreControllerDeviceState not found"
+                    Display --indent 6 --text "- Restore controller device state" --result "NOT FOUND" --color WHITE
+                    AddHP 0 1
+                fi
+                LogText "Checking USBGuard rule for controllers connected before daemon starts (PresentControllerPolicy)"
+                USBGUARD_CONTROLLER_POLICY=$(${AWKBINARY} -F '=' -v OPT="PresentControllerPolicy" 'index($0, OPT) == 1 {print $2}' ${USBGUARD_CONFIG})
+                if [ ! -z "${USBGUARD_CONTROLLER_POLICY}" ]; then
+                    LogText "Result: PresentControllerPolicy = ${USBGUARD_CONTROLLER_POLICY}"
+                    case "${USBGUARD_CONTROLLER_POLICY}" in
+                        "allow"|"keep")
+                            Display --indent 6 --text "- Rule for controllers connected before daemon starts" --result "${USBGUARD_CONTROLLER_POLICY}" --color YELLOW
+                            LogText "  Consider changing PresentControllerPolicy to \"apply-policy\", \"block\" or \"reject\""
+                            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                            # ReportSuggestion ${TEST_NO} "Consider hardening USBGuard configuration" "PresentControllerPolicy (${USBGUARD_CONTROLLER_POLICY} --&gt; (apply-policy|block|reject)"
+                            AddHP 0 1
+                            ;;
+                        "apply-policy"|"block"|"reject")
+                            Display --indent 6 --text "- Rule for controllers connected before daemon starts" --result "${USBGUARD_CONTROLLER_POLICY}" --color GREEN
+                            AddHP 1 1
+                            ;;
+                        *)
+                            LogText "Result: Invalid configuration for PresentControllerPolicy"
+                            Display --indent 6 --text "- Rule for controllers connected before daemon starts" --result "Invalid" --color RED
+                            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                            # ReportSuggestion ${TEST_NO} "Fix USBGuard configuration" "PresentControllerPolicy invalid \"${USBGUARD_CONTROLLER_POLICY}\""
+                            AddHP 0 1
+                            ;;
+                    esac
+                else
+                    LogText "Result: PresentControllerPolicy not found"
+                    Display --indent 6 --text "- Rule for controllers connected before daemon starts" --result "NOT FOUND" --color WHITE
+                    AddHP 0 1
+                fi
+                LogText "Checking USBGuard rule for devices connected before daemon starts (PresentDevicePolicy)"
+                USBGUARD_DEVICE_POLICY=$(${AWKBINARY} -F '=' -v OPT="PresentDevicePolicy" 'index($0, OPT) == 1 {print $2}' ${USBGUARD_CONFIG})
+                if [ ! -z "${USBGUARD_DEVICE_POLICY}" ]; then
+                    LogText "Result: PresentDevicePolicy = ${USBGUARD_DEVICE_POLICY}"
+                    case "${USBGUARD_DEVICE_POLICY}" in
+                        "allow"|"keep")
+                            Display --indent 6 --text "- Rule for devices connected before daemon starts" --result "${USBGUARD_DEVICE_POLICY}" --color YELLOW
+                            LogText "  Consider changing PresentDevicePolicy to \"apply-policy\", \"block\" or \"reject\""
+                            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                            # ReportSuggestion ${TEST_NO} "Consider hardening USBGuard configuration" "PresentDevicePolicy (${USBGUARD_DEVICE_POLICY} --&gt; (apply-policy|block|reject)"
+                            AddHP 0 1
+                            ;;
+                        "apply-policy"|"block"|"reject")
+                            Display --indent 6 --text "- Rule for devices connected before daemon starts" --result "${USBGUARD_DEVICE_POLICY}" --color GREEN
+                            AddHP 1 1
+                            ;;
+                        *)
+                            LogText "Result: Invalid configuration for PresentDevicePolicy"
+                            Display --indent 6 --text "- Rule for devices connected before daemon starts" --result "Invalid" --color RED
+                            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                            # ReportSuggestion ${TEST_NO} "Fix USBGuard configuration" "PresentDevicePolicy invalid \"${USBGUARD_DEVICE_POLICY}\""
+                            AddHP 0 1
+                            ;;
+                    esac
+                else
+                    LogText "Result: PresentDevicePolicy not found"
+                    Display --indent 6 --text "- Rule for devices connected before daemon starts" --result "NOT FOUND" --color WHITE
+                    AddHP 0 1
+                fi
+                LogText "Checking USBGuard rule for devices inserted after daemon starts (InsertedDevicePolicy)"
+                USBGUARD_INSERTED_POLICY=$(${AWKBINARY} -F '=' -v OPT="InsertedDevicePolicy" 'index($0, OPT) == 1 {print $2}' ${USBGUARD_CONFIG})
+                if [ ! -z "${USBGUARD_INSERTED_POLICY}" ]; then
+                    LogText "Result: InsertedDevicePolicy = ${USBGUARD_INSERTED_POLICY}"
+                    case "${USBGUARD_INSERTED_POLICY}" in
+                        "allow"|"keep")
+                            Display --indent 6 --text "- Rule for devices inserted after daemon starts" --result "${USBGUARD_INSERTED_POLICY}" --color YELLOW
+                            LogText "  Consider changing InsertedDevicePolicy to \"apply-policy\", \"block\" or \"reject\""
+                            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                            # ReportSuggestion ${TEST_NO} "Consider hardening USBGuard configuration" "InsertedDevicePolicy (${USBGUARD_INSERTED_POLICY} --&gt; (apply-policy|block|reject)"
+                            AddHP 0 1
+                            ;;
+                        "apply-policy"|"block"|"reject")
+                            Display --indent 6 --text "- Rule for devices inserted after daemon starts" --result "${USBGUARD_INSERTED_POLICY}" --color GREEN
+                            AddHP 1 1
+                            ;;
+                        *)
+                            LogText "Result: Invalid configuration for InsertedDevicePolicy"
+                            Display --indent 6 --text "- Rule for devices inserted after daemon starts" --result "Invalid" --color RED
+                            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                            # ReportSuggestion ${TEST_NO} "Fix USBGuard configuration" "InsertedDevicePolicy invalid \"${USBGUARD_INSERTED_POLICY}\""
+                            AddHP 0 1
+                            ;;
+                    esac
+                else
+                    LogText "Result: InsertedDevicePolicy not found"
+                    Display --indent 6 --text "- Rule for devices inserted after daemon starts" --result "NOT FOUND" --color WHITE
+                    AddHP 0 1
+                fi
+                LogText "Checking USBGuard rule for devices not in RuleFile (ImplicitPolicyTarget)"
+                USBGUARD_DEFAULT_POLICY=$(${AWKBINARY} -F '=' -v OPT="ImplicitPolicyTarget" 'index($0, OPT) == 1 {print $2}' ${USBGUARD_CONFIG})
+                if [ ! -z "${USBGUARD_DEFAULT_POLICY}" ]; then
+                    LogText "Result: ImplicitPolicyTarget = ${USBGUARD_DEFAULT_POLICY}"
+                    case "${USBGUARD_DEFAULT_POLICY}" in
+                        "allow")
+                            Display --indent 6 --text "- Rule for devices not in RuleFile" --result "${USBGUARD_DEFAULT_POLICY}" --color YELLOW
+                            LogText "  Consider changing ImplicitPolicyTarget to \"block\" or \"reject\""
+                            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                            # ReportSuggestion ${TEST_NO} "Consider hardening USBGuard configuration" "ImplicitPolicyTarget (${USBGUARD_DEFAULT_POLICY} --&gt; (block|reject)"
+                            AddHP 0 1
+                            ;;
+                        "block"|"reject")
+                            Display --indent 6 --text "- Rule for devices not in RuleFile" --result "${USBGUARD_DEFAULT_POLICY}" --color GREEN
+                            AddHP 1 1
+                            ;;
+                        *)
+                            LogText "Result: Invalid configuration for ImplicitPolicyTarget"
+                            Display --indent 6 --text "- Rule for devices not in RuleFile" --result "Invalid" --color RED
+                            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                            # ReportSuggestion ${TEST_NO} "Fix USBGuard configuration" "ImplicitPolicyTarget invalid \"${USBGUARD_DEFAULT_POLICY}\""
+                            AddHP 0 1
+                            ;;
+                    esac
+                else
+                    LogText "Result: ImplicitPolicyTarget not found"
+                    Display --indent 4 --text "- Rule for devices not in RuleFile" --result "NOT FOUND" --color WHITE
+                    AddHP 0 1
+                fi
+                LogText "Checking RuleFile"
+                USBGUARD_RULES=$(${AWKBINARY} -F '=' -v OPT="RuleFile" 'index($0, OPT) == 1 {print $2}' ${USBGUARD_CONFIG})
+                if [ ! -z "${USBGUARD_RULES}" ] &amp;&amp; [ -f "${USBGUARD_RULES}" ]; then
+                    LogText "Result: RuleFile found (${USBGUARD_RULES})"
+                    Display --indent 4 --text "- RuleFile" --result "${STATUS_FOUND}" --color GREEN
+                    AddHP 1 1
+                    USBGUARD_RULES_ALLOW=$(${EGREPBINARY} -c "^allow" ${USBGUARD_RULES})
+                    Display --indent 6 --text "- Controllers &amp; Devices allow" --result "${USBGUARD_RULES_ALLOW}" --color WHITE
+                    USBGUARD_RULES_BLOCK=$(${EGREPBINARY} -c "^block" ${USBGUARD_RULES})
+                    Display --indent 6 --text "- Controllers &amp; Devices block" --result "${USBGUARD_RULES_BLOCK}" --color WHITE
+                    USBGUARD_RULES_REJECT=$(${EGREPBINARY} -c "^reject" ${USBGUARD_RULES})
+                    Display --indent 6 --text "- Controllers &amp; Devices reject" --result "${USBGUARD_RULES_REJECT}" --color WHITE
+                else
+                    LogText "Result: RuleFile not found (\"man usbguard\" for instructions to install initial policies)"
+                    Display --indent 4 --text "- RuleFile" --result "${STATUS_NOT_FOUND}" --color RED
+                    # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                    #ReportSuggestion ${TEST_NO} "Install USBGuard RuleFile" "\"man usbguard\" for instructions to install initial policies"
+                    AddHP 0 1
+                fi
+            else
+                Display --indent 4 --text "- Configuration" --result "${STATUS_NOT_FOUND}" --color WHITE
+                LogText "Result: Configuration not found"
+                # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+                #ReportSuggestion ${TEST_NO} "USBGuard configuration file not found, consider reinstalling"
+                AddHP 0 7
+            fi
+        else
+            LogText "Result: USBGuard not found"
+            Display --indent 2 --text "- Checking USBGuard" --result "${STATUS_NOT_FOUND}" --color WHITE
+            # To-Be-Added: assign TEST_NO, create documentation, and enable the suggestion
+            #ReportSuggestion ${TEST_NO} "Install USBGuard to allow for fine-grained control of USB authorization"
+            AddHP 0 8
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>#    # Test        : VIRT-1920
+#    # Description : Checking VMware
+#    Register --test-no VIRT-1920 --weight L --network NO --category security --description "Checking VMware guest status"
+#    if [ ${SKIPTEST} -eq 0 ]; then
+#        # Initialise
+#        VMWARE_GUEST=0
+#        Display --indent 2 --text "- Checking VMware guest status"
+#        # check memory driver file
+#        # check LKM list
+#        # check vmware tools
+#        LogText "Test: checking VMware tools daemon presence"
+#        if [ ! "${VMWARETOOLSBINARY}" = "" ]; then
+#            LogText "Result: VMware tools binary found"
+#            VMWARE_GUEST=1
+#            Display --indent 4 --text "- Checking VMware tools daemon" --result "${STATUS_FOUND}" --color GREEN
+#          else
+#            Display --indent 4 --text "- Checking VMware tools daemon" --result "${STATUS_NOT_FOUND}" --color WHITE
+#        fi
+#
+#    fi
+#</t>
+  </si>
+  <si>
+    <t>Apache installatin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6622
+    # Description : Test for Apache installation
+    # Notes       : Do not run on NetBSD, -v is unknown option for httpd binary
+    #               On OpenBSD do not run /usr/sbin/httpd with -v: builtin non-Apache
+    if [ ! "${OS}" = "NetBSD" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6622 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Checking Apache presence"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        if [ "${OS}" = "OpenBSD" -a "${HTTPDBINARY}" = "/usr/sbin/httpd" ]; then HTTPDBINARY=""; fi
+        if IsEmpty "${HTTPDBINARY}"; then
+            Display --indent 2 --text "- Checking Apache" --result "${STATUS_NOT_FOUND}" --color WHITE
+        else
+            LogText "Test: Scanning for Apache binary"
+            IS_APACHE=$(${HTTPDBINARY} -v 2&gt; /dev/null | ${EGREPBINARY} '[aA]pache')
+            if IsEmpty "${IS_APACHE}"; then
+                LogText "Result: ${HTTPDBINARY} is not Apache"
+                Display --indent 2 --text "- Checking Apache (binary ${HTTPDBINARY})" --result "NO MATCH" --color WHITE
+            else
+                Display --indent 2 --text "- Checking Apache (binary ${HTTPDBINARY})" --result "${STATUS_FOUND}" --color GREEN
+                LogText "Result: ${HTTPDBINARY} seems to be Apache HTTP daemon"
+                APACHE_INSTALLED=1
+                APACHE_VERSION=$(${HTTPDBINARY} -v 2&gt; /dev/null | ${GREPBINARY} "^Server version:" | ${AWKBINARY} '{ print $3 }' | ${AWKBINARY} -F/ '{ print $2 }')
+                LogText "Apache version: ${APACHE_VERSION}"
+                Report "apache_version=${APACHE_VERSION}"
+            fi
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>Main Apache config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6624
+    # Description : Testing main Apache configuration file
+    # Notes       : Do not run on OpenBSD/NetBSD, as -V is an unknown option for httpd binary
+    if [ ${APACHE_INSTALLED} -eq 1 ]; then
+        if [ ! "${OS}" = "NetBSD" -a ! "${OS}" = "OpenBSD" ]; then
+            PREQS_MET="YES"
+        else
+            PREQS_MET="NO"
+        fi
+    else
+        PREQS_MET="NO"
+    fi
+    Register --test-no HTTP-6624 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Testing main Apache configuration file"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        APACHE_CONFIGFILE=""
+        APACHE_TEST=$(${HTTPDBINARY} -V 2&gt; /dev/null | ${GREPBINARY} "\-D SERVER_CONFIG_FILE=" | ${SEDBINARY} 's/[ ]-D SERVER_CONFIG_FILE=//' | ${TRBINARY} -d '"' | ${TRBINARY} -d ' ' | ${TRBINARY} -d '[:cntrl:]')
+        if IsEmpty "${APACHE_TEST}"; then
+            LogText "Result: Can't find the configuration file, so skipping some Apache related tests"
+        else
+            # We found a possible match. Checking if it's valid filename. If not, we need to add a prefix
+            if [ -f ${APACHE_TEST} ]; then
+                APACHE_CONFIGFILE="${APACHE_TEST}"
+                Display --indent 6 --text "Info: Configuration file found (${APACHE_CONFIGFILE})"
+            else
+                # Probably the prefix is missing, so we are going to search that
+                APACHE_HTTPDROOT=$(${HTTPDBINARY} -V 2&gt; /dev/null | ${GREPBINARY} "\-D HTTPD_ROOT=" | ${SEDBINARY} 's/[ ]-D HTTPD_ROOT=//' | ${TRBINARY} -d '"' | ${TRBINARY} -d ' ')
+                APACHE_TESTFILE="${APACHE_HTTPDROOT}/${APACHE_TEST}"
+                if [ -f ${APACHE_TESTFILE} ]; then
+                    APACHE_CONFIGFILE="${APACHE_TESTFILE}"
+                    Display --indent 6 --text "Info: Configuration file found (${APACHE_CONFIGFILE})"
+                    LogText "Result: Configuration file found (${APACHE_CONFIGFILE})"
+                else
+                    LogText "Result: File or directory ${APACHE_CONFIGFILE} does not exist"
+                    Display --indent 6 --text "[Notice] possible directory/file parts found, but still unsure what the real configuration file is. Skipping some Apache related tests"
+                    ReportException "${TEST_NO}:1" "Found some unknown directory or file references in Apache configuration"
+                fi
+            fi
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>Other Apache configs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6626
+    # Description : Testing other Apache configuration files
+    if [ ${APACHE_INSTALLED} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6626 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Testing other Apache configuration file"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        for DIR in ${sTEST_APACHE_TARGETS}; do
+            if [ -d ${DIR} ]; then
+                find ${DIR} -name "*.conf" -print &gt;&gt; ${TMPFILE2}
+            fi
+        done
+        # Sort unsorted list, save it in temp file and then remove unsorted list
+        if [ -f ${TMPFILE2} ]; then
+            ${SORTBINARY} -u ${TMPFILE2} &gt;&gt; ${TMPFILE}
+            rm -f ${TMPFILE2}
+        fi
+        cVHOSTS=0; tVHOSTS=""
+        # Check every configuration file
+        for I in $(cat ${TMPFILE}); do
+            LogText "Apache config file: ${I}"
+            FileIsReadable ${I}
+            if [ ${CANREAD} -eq 1 ]; then
+                # Search Virtual Hosts
+                for J in $(${GREPBINARY} "ServerName" ${I} | ${GREPBINARY} -v "^#" | ${AWKBINARY} '{ if ($1=="ServerName" &amp;&amp; $2!="*" &amp;&amp; $2!="default") print $2 }'); do
+                    if HasData "${J}"; then
+                        tVHOSTS="${tVHOSTS} ${J}"
+                        cVHOSTS=$((cVHOSTS + 1))
+                    fi
+                done
+                # Search Server aliases
+                for J in $(${GREPBINARY} "ServerAlias" ${I} | ${GREPBINARY} -v "^#" | ${SEDBINARY} "s/\s*ServerAlias //g" | ${SEDBINARY} "s/#.*//g"); do
+                    if [ ! -z ${J} ]; then
+                        tVHOSTS="${tVHOSTS} ${J}"
+                        cVHOSTS=$((cVHOSTS + 1))
+                    fi
+                done
+            else
+                LogText "Result: can not read configuration file with this user ID"
+                ReportException "${TEST_NO}:1" "Can not read configuration file $I"
+            fi
+        done
+        # Log all virtual hosts we found
+            for J in ${tVHOSTS}; do
+                if [ ! -z ${J} ]; then
+                    LogText "Virtual host: ${J}"
+                    Report "apache_vhost_name[]=${J}"
+                fi
+            done
+        # Show number of vhosts if we found any
+        LogText "Result: found ${cVHOSTS} virtual hosts"
+        if [ ${cVHOSTS} -gt 0 ]; then
+            Display --indent 6 --text "Info: Found ${cVHOSTS} virtual hosts"
+        else
+            Display --indent 6 --text "Info: No virtual hosts found"
+        fi
+    fi
+    # Remove temp files
+    if [ -f ${TMPFILE} -a ! -z "${TMPFILE}" ]; then
+        rm -f ${TMPFILE}
+    fi
+    if [ ! -z "${TMPFILE2}" ]; then if [ -f ${TMPFILE2} ]; then rm -f ${TMPFILE2}; fi; fi
+#</t>
+  </si>
+  <si>
+    <t>Apache loaded modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # TODO
+    # Do you have Apache running and want to contribute? Help us testing this control and send in a pull request
+    # Test        : HTTP-6630
+    # Description : Search for all loaded modules
+    #if [ ${APACHE_INSTALLED} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    #Register --test-no HTTP-6630 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Determining all loaded Apache modules"
+    #if [ ${SKIPTEST} -eq 0 ]; then
+    #    # Testing Debian style
+    #    LogText "Test: searching loaded/enabled Apache modules"
+    #    apachectl -t -D DUMP_MODULES 2&gt;&amp;1 | ${EGREPBINARY} -v "(Loaded Modules|Syntax OK)" | ${SEDBINARY} 's/(\(shared\|static\))//' | ${SEDBINARY} 's/ //'
+    #    for I in ${APACHE_MODULES_ENABLED_LOCS}; do
+    #        LogText "Test: checking ${I}"
+    #        if [ -d ${I} ]; then
+    #            FIND=$(${GREPBINARY} -r LoadModule ${I}/* | ${GREPBINARY} -v "^#" | ${AWKBINARY} '{ print $2":"$3 }')
+    #          else
+    #            LogText "Result: ${I} does not exist"
+    #        fi
+    #    done
+    #fi
+#</t>
+  </si>
+  <si>
+    <t>Available Apache modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6632
+    # Description : Search for available Apache modules
+    if [ ${APACHE_INSTALLED} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6632 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Determining all available Apache modules"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: searching available Apache modules"
+        COUNT=0
+        for DIR in ${APACHE_MODULES_LOCS}; do
+            DirectoryExists ${DIR}
+            if [ ${DIRECTORY_FOUND} -eq 1 ]; then
+                FIND=$(${FINDBINARY} ${DIR} -name "mod_*" -print | ${SORTBINARY})
+                for ITEM in ${FIND}; do
+                    Report "apache_module[]=${ITEM}"
+                    LogText "Result: found Apache module ${ITEM}"
+                    COUNT=$((COUNT + 1))
+                done
+            fi
+        done
+        if [ ${COUNT} -eq 0 ]; then
+            Display --indent 4 --text "* Loadable modules" --result "${STATUS_NONE}" --color WHITE
+            ReportException "${TEST_NO}:1" "No loadable Apache modules found"
+        else
+            Display --indent 4 --text "* Loadable modules" --result "${STATUS_FOUND} (${COUNT})" --color GREEN
+            Display --indent 8 --text "- Found ${COUNT} loadable modules"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>Module: evasive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6640
+    # Description : Search for special Apache modules: evasive
+    if [ ${APACHE_INSTALLED} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6640 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Determining existence of specific Apache modules"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        # Check modules, module
+        CheckItem "apache_module" "/mod_evasive([0-9][0-9])?.so"
+        if [ ${ITEM_FOUND} -eq 1 ]; then
+            Display --indent 10 --text "mod_evasive: anti-DoS/brute force" --result "${STATUS_FOUND}" --color GREEN
+            AddHP 3 3
+        else
+            Display --indent 10 --text "mod_evasive: anti-DoS/brute force" --result "${STATUS_NOT_FOUND}" --color WHITE
+            AddHP 2 3
+            ReportSuggestion ${TEST_NO} "Install Apache mod_evasive to guard webserver against DoS/brute force attempts"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>Module: QoS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6641
+    # Description : Search for special Apache modules: Quality of Service
+    # Notes       : Was mod_qos before. Since Apache 2.2.15 mod_reqtimeout
+    if [ ${APACHE_INSTALLED} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6641 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Determining existence of specific Apache modules"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        # Check modules, module
+        CheckItem "apache_module" "/mod_(reqtimeout|qos).so"
+        if [ ${ITEM_FOUND} -eq 1 ]; then
+            Display --indent 10 --text "mod_reqtimeout/mod_qos" --result "${STATUS_FOUND}" --color GREEN
+            AddHP 3 3
+        else
+            Display --indent 10 --text "mod_reqtimeout/mod_qos" --result "${STATUS_NOT_FOUND}" --color WHITE
+            AddHP 2 3
+            ReportSuggestion ${TEST_NO} "Install Apache mod_reqtimeout or mod_qos to guard webserver against Slowloris attacks"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>Module: security</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6643
+    # Description : Search for special Apache modules: security
+    if [ ${APACHE_INSTALLED} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6643 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Determining existence of specific Apache modules"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        # Check modules, module
+        CheckItem "apache_module" "/mod_security2.so"
+        if [ ${ITEM_FOUND} -eq 1 ]; then
+            Display --indent 10 --text "ModSecurity: web application firewall" --result "${STATUS_FOUND}" --color GREEN
+            AddHP 3 3
+        else
+            Display --indent 10 --text "ModSecurity: web application firewall" --result "${STATUS_NOT_FOUND}" --color WHITE
+            AddHP 2 3
+            ReportSuggestion ${TEST_NO} "Install Apache modsecurity to guard webserver against web application attacks"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>TraceEnable off in config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6660 TODO
+    # Description : Search for "TraceEnable off" in configuration files
+#</t>
+  </si>
+  <si>
+    <t>nginx process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6702
+    # Description : Search for nginx process
+    Register --test-no HTTP-6702 --weight L --network NO --category security --description "Check nginx process"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: searching running nginx process"
+        if IsRunning "nginx"; then
+            LogText "Result: found running nginx process(es)"
+            Display --indent 2 --text "- Checking nginx" --result "${STATUS_FOUND}" --color GREEN
+            NGINX_RUNNING=1
+            Report "nginx_running=1"
+        else
+            LogText "Result: no running nginx process found"
+            Display --indent 2 --text "- Checking nginx" --result "${STATUS_NOT_FOUND}" --color WHITE
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>nginx config</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6704
+    # Description : Search for nginx configuration file
+    if [ ${NGINX_RUNNING} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6704 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check nginx configuration file"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: searching nginx configuration file"
+        for DIR in ${NGINX_CONF_LOCS}; do
+            if [ -f ${DIR}/nginx.conf ]; then
+                NGINX_CONF_LOCATION="${DIR}/nginx.conf"
+                LogText "Found file ${NGINX_CONF_LOCATION}"
+                NGINX_CONF_FILES="${DIR}/nginx.conf"
+            fi
+        done
+        if HasData "${NGINX_CONF_LOCATION}"; then
+            LogText "Result: found nginx configuration file"
+            Report "nginx_main_conf_file=${NGINX_CONF_LOCATION}"
+            Display --indent 4 --text "- Searching nginx configuration file" --result "${STATUS_FOUND}" --color GREEN
+        else
+            LogText "Result: no nginx configuration file found"
+            Display --indent 2 --text "- Searching nginx configuration file" --result "${STATUS_NOT_FOUND}" --color WHITE
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>nginx includes</t>
+  </si>
+  <si>
+    <t>#
+    # Test        : HTTP-6706
+    # Description : Search for includes within nginx configuration file
+    # Notes       : Daemon nginx should be running, nginx.conf should be found
+    if [ ${NGINX_RUNNING} -eq 1 -a ! -z "${NGINX_CONF_LOCATION}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6706 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check for additional nginx configuration files"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        CreateTempFile || ExitFatal
+        TMPFILE="${TEMP_FILE}"
+        COUNT=0
+        ${SEDBINARY} -e 's/^[ \t]*//' ${NGINX_CONF_LOCATION} | ${GREPBINARY} -v "^#" | ${GREPBINARY} -v "^$" | ${SEDBINARY} 's/[\t]/ /g' | ${SEDBINARY} 's/  / /g' | ${SEDBINARY} 's/  / /g' &gt;&gt; ${TMPFILE}
+        # Search for included configuration files (may include directories and wild cards)
+        FIND=$(${GREPBINARY} "include" ${NGINX_CONF_LOCATION} | ${AWKBINARY} '{ if ($1=="include") { print $2 }}' | ${SEDBINARY} 's/;$//g')
+        for I in ${FIND}; do
+            FIND2=$(${LSBINARY} ${I} 2&gt;/dev/null)
+            for J in ${FIND2}; do
+                # Ensure that we are parsing normal files
+                if [ -f ${J} ]; then
+                    COUNT=$((COUNT + 1))
+                    LogText "Result: found Nginx configuration file ${J}"
+                    Report "nginx_sub_conf_file[]=${J}"
+                    FileIsReadable ${J}
+                    if [ ${CANREAD} -eq 1 ]; then
+                        NGINX_CONF_FILES="${NGINX_CONF_FILES} ${J}"
+                        FIND3=$(sed -e 's/^[ \t]*//' ${J} | ${GREPBINARY} -v "^#" | ${GREPBINARY} -v "^$" | ${SEDBINARY} 's/[\t]/ /g' | ${SEDBINARY} 's/  / /g' | ${SEDBINARY} 's/  / /g' &gt;&gt; ${TMPFILE})
+                    else
+                        ReportException "${TEST_NO}:1" "Can not parse file ${J}, as it is not readable"
+                    fi
+                fi
+            done
+        done
+        # Sort all discovered configuration lines and store unique ones. Also strip out the mime types configured in nginx
+        SORTFILE=$(${SORTBINARY} -u ${TMPFILE} | ${SEDBINARY} 's/ /:space:/g' | ${EGREPBINARY} -v "(application|audio|image|text|video)/" | ${EGREPBINARY} -v "({|})")
+        for I in ${SORTFILE}; do
+            I=$(echo ${I} | ${SEDBINARY} 's/:space:/ /g')
+            Report "nginx_config_option[]=${I}";
+        done
+        # Remove unsorted file for next tests
+        if [ -f ${TMPFILE} ]; then rm -f ${TMPFILE}; fi
+        if [ ${COUNT} -eq 0 ]; then
+            LogText "Result: no nginx include statements found"
+        else
+            Display --indent 6 --text "- Found nginx includes" --result "${COUNT} FOUND" --color GREEN
+        fi
+    fi</t>
+  </si>
+  <si>
+    <t>nginx configs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6708
+    # Description : Check discovered nginx configuration settings for further hardening
+    # Notes       : Daemon of nginx should be running, nginx.conf should be found
+    if [ ${NGINX_RUNNING} -eq 1 -a ! -z "${NGINX_CONF_FILES}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6708 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check discovered nginx configuration settings"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: start parsing all discovered nginx options"
+        Display --indent 4 --text "- Parsing configuration options"
+        for FILE in ${NGINX_CONF_FILES}; do
+            FILENAME=$(echo ${FILE} | ${AWKBINARY} -F/ '{print $NF}')
+            if [ ! "${FILENAME}" = "mime.types" ]; then
+                if FileIsReadable ${FILE}; then
+                    Display --indent 8 --text "- ${FILE}"
+                    ParseNginx ${FILE}
+                else
+                    Display --indent 8 --text "- ${FILE}" --result "SKIPPED (NOT READABLE)" --color YELLOW
+                fi
+            else
+                LogText "Result: this configuration file is skipped, as it contains usually no interesting details"
+            fi
+        done
+        if [ ! -z "${NGINX_CONF_FILES_ADDITIONS}" ]; then
+            for I in ${NGINX_CONF_FILES_ADDITIONS}; do
+                FILENAME=$(echo ${I} | ${AWKBINARY} -F/ '{print $NF}')
+                if [ ! "${FILENAME}" = "mime.types" ]; then
+                    if FileIsReadable ${I}; then
+                        Display --indent 8 --text "- ${I}"
+                        ParseNginx ${I}
+                    else
+                        Display --indent 8 --text "- ${I}" --result "SKIPPED (NOT READABLE)" --color YELLOW
+                    fi
+                else
+                    LogText "Result: this configuration file is skipped, as it contains usually no interesting details"
+                fi
+            done
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>nginx ssl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6710
+    # Description : Check SSL configuration of nginx
+    # Notes       : Daemon of nginx should be running, nginx.conf should be found
+    if [ ${NGINX_RUNNING} -eq 1 -a ! -z "${NGINX_CONF_LOCATION}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6710 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check nginx SSL configuration settings"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        NGINX_SSL_SUGGESTION=0
+        if [ ${NGINX_SSL_ON} -eq 1 ]; then
+            LogText "Result: SSL is configured in nginx on one or more virtual hosts"
+            Display --indent 6 --text "- SSL configured" --result "${STATUS_YES}" --color GREEN
+            AddHP 5 5
+            # Cipher tests
+            if [ ${NGINX_SSL_CIPHERS} -eq 1 ]; then
+                Display --indent 8 --text "- Ciphers configured" --result "${STATUS_YES}" --color GREEN
+            else
+                Display --indent 8 --text "- Ciphers configured" --result "${STATUS_NO}" --color RED
+                NGINX_SSL_SUGGESTION=1
+            fi
+            if [ ${NGINX_SSL_PREFER_SERVER_CIPHERS} -eq 1 ]; then
+                Display --indent 8 --text "- Prefer server ciphers" --result "${STATUS_YES}" --color GREEN
+            else
+                Display --indent 8 --text "- Prefer server ciphers" --result "${STATUS_NO}" --color RED
+                NGINX_SSL_SUGGESTION=1
+            fi
+            if [ ${NGINX_SSL_PROTOCOLS} -eq 1 ]; then
+                Display --indent 8 --text "- Protocols configured" --result "${STATUS_YES}" --color GREEN
+                if [ ${NGINX_WEAK_SSL_PROTOCOL_FOUND} -eq 0 ]; then
+                    Display --indent 10 --text "- Insecure protocols found" --result "${STATUS_NO}" --color GREEN
+                else
+                    Display --indent 10 --text "- Insecure protocols found" --result "${STATUS_YES}" --color RED
+                    ReportSuggestion "${TEST_NO}" "Disable weak protocol in nginx configuration"
+                fi
+            else
+                Display --indent 8 --text "- Protocols configured" --result "${STATUS_NO}" --color RED
+                NGINX_SSL_SUGGESTION=1
+            fi
+        else
+            LogText "Result: No SSL configuration found"
+            Display --indent 6 --text "- SSL configured" --result "${STATUS_NO}" --color RED
+            ReportSuggestion ${TEST_NO} "Add HTTPS to nginx virtual hosts for enhanced protection of sensitive data and privacy"
+            AddHP 1 5
+        fi
+        if [ ${NGINX_SSL_SUGGESTION} -eq 1 ]; then
+            LogText "Result: one or more parts of the nginx configuration could be enhanced regarding SSL"
+            ReportSuggestion "${TEST_NO}" "Change the HTTPS and SSL settings for enhanced protection of sensitive data and privacy"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>nginx logging</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6712
+    # Description : Check logging configuration of nginx
+    # Notes       : Daemon of nginx should be running, nginx.conf should be found
+    if [ ${NGINX_RUNNING} -eq 1 -a ! -z "${NGINX_CONF_LOCATION}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6712 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check nginx access logging"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        NGINX_LOG_SUGGESTION=0
+        Display --indent 6 --text "- Checking log file configuration"
+        # Check for missing access log
+        if [ ${NGINX_ACCESS_LOG_MISSING} -eq 1 ]; then
+            NGINX_LOG_SUGGESTION=1
+            Display --indent 8 --text "- Missing log files (access_log)" --result "${STATUS_YES}" --color RED
+        else
+            Display --indent 8 --text "- Missing log files (access_log)" --result "${STATUS_NO}" --color GREEN
+        fi
+        # Access log disabled
+        if [ ${NGINX_ACCESS_LOG_DISABLED} -eq 1 ]; then
+            NGINX_LOG_SUGGESTION=1
+            LogText "Result: found one or more virtual hosts which have their access log disabled"
+            Display --indent 8 --text "- Disabled access logging" --result "${STATUS_YES}" --color RED
+            AddHP 2 3
+        else
+            LogText "Result: no virtual hosts found which have their access log disabled"
+            Display --indent 8 --text "- Disabled access logging" --result "${STATUS_NO}" --color GREEN
+            AddHP 3 3
+        fi
+        # Report suggestion
+        if [ ${NGINX_LOG_SUGGESTION} -eq 1 ]; then
+            ReportSuggestion ${TEST_NO} "Check your nginx access log for proper functioning"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>nginx missing error logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6714
+    # Description : Check missing error logs in nginx
+    if [ ${NGINX_RUNNING} -eq 1 -a ! -z "${NGINX_CONF_LOCATION}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6714 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check for missing error logs in nginx"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        NGINX_LOG_SUGGESTION=0
+        # Check for missing access log
+        if [ ${NGINX_ERROR_LOG_MISSING} -eq 1 ]; then
+            NGINX_LOG_SUGGESTION=1
+            Display --indent 8 --text "- Missing log files (error_log)" --result "${STATUS_YES}" --color RED
+        else
+            Display --indent 8 --text "- Missing log files (error_log)" --result "${STATUS_NO}" --color GREEN
+        fi
+        # Report suggestion
+        if [ ${NGINX_LOG_SUGGESTION} -eq 1 ]; then
+            ReportSuggestion ${TEST_NO} "Check your nginx error_log statements"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>nginx error log debug mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Test        : HTTP-6716
+    # Description : Check debug mode on error log in nginx
+    if [ ${NGINX_RUNNING} -eq 1 -a ! -z "${NGINX_CONF_LOCATION}" ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6716 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check for debug mode on error log in nginx"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        NGINX_LOG_SUGGESTION=0
+        # Access log in debug mode
+        if [ ${NGINX_ERROR_LOG_DEBUG} -eq 1 ]; then
+            NGINX_LOG_SUGGESTION=1
+            LogText "Result: found one or more virtual hosts which have their error log in debug mode"
+            Display --indent 8 --text "- Debugging mode on error_log" --result "${STATUS_YES}" --color RED
+            AddHP 2 3
+        else
+            LogText "Result: no virtual hosts found which have their error log in debug mode"
+            Display --indent 8 --text "- Debugging mode on error_log" --result "${STATUS_NO}" --color GREEN
+            AddHP 3 3
+        fi
+        # Report suggestion
+        if [ ${NGINX_LOG_SUGGESTION} -eq 1 ]; then
+            ReportSuggestion ${TEST_NO} "Check your nginx error_log statements and disable debug mode"
+        fi
+    fi
+#</t>
+  </si>
+  <si>
+    <t>nginx log files</t>
+  </si>
+  <si>
+    <t>#
+    # Test        : HTTP-6720
+    # Description : Search for nginx log files
+    if [ ${NGINX_RUNNING} -eq 1 ]; then PREQS_MET="YES"; else PREQS_MET="NO"; fi
+    Register --test-no HTTP-6720 --preqs-met ${PREQS_MET} --weight L --network NO --category security --description "Check Nginx log files"
+    if [ ${SKIPTEST} -eq 0 ]; then
+        LogText "Test: Checking directories for files with log file definitions"
+        for DIR in ${NGINX_CONF_LOCS}; do
+            LogText "Test: Checking ${DIR}"
+            if [ -d ${DIR} ]; then
+                LogText "Result: Directory ${DIR} exists, so will be used as search path"
+                FIND=$(find ${DIR} -type f -exec ${GREPBINARY} access_log \{\} \; | ${GREPBINARY} -v "#" | ${AWKBINARY} '{ if($1=="access_log") { print $2 } }' | ${SEDBINARY} 's/;$//g' | ${SORTBINARY} -u)
+                if IsEmpty "${FIND}"; then
+                    LogText "Result: no log files found"
+                else
+                    LogText "Result: found one or more log files"
+                    for FILE in ${FIND}; do
+                        if [ -f ${FILE} ]; then
+                            LogText "Found log file: ${FILE}"
+                            Report "log_file=${FILE}"
+                        else
+                            LogText "Found non existing log file: ${FILE}"
+                        fi
+                    done
+                fi
+            else
+                LogText "Result: directory ${DIR} not found, skipping search in this directory."
+            fi
+        done
+        unset DIR; unset FILE; unset FIND
+    fi
+#</t>
+  </si>
+  <si>
+    <t>Tips when enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    # Only show tips when enabled
+    if [ ${SHOW_TOOL_TIPS} -eq 1 ]; then
+        # Bash completion support
+        if [ ! "${ETC_PATHS}" = "" ]; then
+            for I in ${ETC_PATHS}; do
+                if [ -d ${I}/bash-completion.d ]; then
+                    if [ ! -f ${ETC_PATHS}/bash_completion.d/lynis ]; then
+                        Display "This system has a bash_completion directory. Copy extras/bash_completion.d/lynis to ${I} to get completion support for Lynis"
+                    fi
+                fi
+            done
         fi
     fi
 #</t>
@@ -17066,7 +20456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
@@ -17402,6 +20792,98 @@
       </c>
       <c r="B42" s="3" t="s">
         <v>1148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="134.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1151</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1157</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1160</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1165</v>
       </c>
     </row>
   </sheetData>
@@ -17548,6 +21030,652 @@
       </c>
       <c r="B16" s="5" t="s">
         <v>517</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="137.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1169</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="136.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1183</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="135.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1184</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="135.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1199</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1202</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1203</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1210</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="136.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1218</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="137.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1220</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="136.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="134" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1236</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="135.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1242</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1244</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1246</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1251</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1252</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1253</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1260</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1263</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="135.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1264</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1268</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1273</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1277</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1278</v>
       </c>
     </row>
   </sheetData>
@@ -17852,6 +21980,267 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="136" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1284</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="136.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>487</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1285</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="135.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1292</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1295</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>1301</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1306</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>1311</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>1318</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>1320</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="99.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="134.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" ht="99.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1322</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1323</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>

</xml_diff>